<commit_message>
If a location is used by two or more terminals, don't try to optimize it away
</commit_message>
<xml_diff>
--- a/src/Sandbox/Comparison.xlsx
+++ b/src/Sandbox/Comparison.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joelv\Desktop\PumpjackPipeOptimizer\src\PumpjackPipeOptimizer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joelv\Desktop\PumpjackPipeOptimizer\src\Sandbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03A34A3-B957-43EE-A637-4F2DEC8824A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3403C635-FD13-44FE-B1F7-2D4F5256B9D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F3EEF332-D963-44B3-89AD-4C5E1973BCE9}"/>
   </bookViews>
@@ -547,7 +547,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -555,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0EBF3A-B501-4205-AA83-0ECFC9C1E5B1}">
-  <dimension ref="A1:W61"/>
+  <dimension ref="A1:X61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
-      <selection activeCell="P44" sqref="P44"/>
+    <sheetView tabSelected="1" topLeftCell="F31" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,7 +568,7 @@
     <col min="18" max="18" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
@@ -633,7 +633,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>20</v>
@@ -699,7 +699,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -771,8 +771,12 @@
         <f>V3-B3</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X3">
+        <f>D3-V3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -844,8 +848,12 @@
         <f t="shared" ref="W4:W60" si="1">V4-B4</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X4">
+        <f t="shared" ref="X4:X60" si="2">D4-V4</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -917,8 +925,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X5">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -990,8 +1002,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X6">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -1063,8 +1079,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X7">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -1136,8 +1156,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X8">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -1209,8 +1233,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X9">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -1282,8 +1310,12 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X10">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -1355,8 +1387,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X11">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -1428,8 +1464,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X12">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -1501,8 +1541,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X13">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -1574,8 +1618,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X14">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -1647,8 +1695,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X15">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -1720,8 +1772,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X16">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -1793,8 +1849,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X17">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -1866,8 +1926,12 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X18">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -1939,8 +2003,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X19">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -2012,8 +2080,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -2085,8 +2157,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X21">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -2158,8 +2234,12 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X22">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -2231,8 +2311,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -2304,8 +2388,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X24">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -2377,8 +2465,12 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X25">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>23</v>
       </c>
@@ -2450,8 +2542,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>24</v>
       </c>
@@ -2523,8 +2619,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>25</v>
       </c>
@@ -2596,8 +2696,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X28">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>26</v>
       </c>
@@ -2669,8 +2773,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>27</v>
       </c>
@@ -2742,8 +2850,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X30">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>28</v>
       </c>
@@ -2815,8 +2927,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X31">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>29</v>
       </c>
@@ -2888,8 +3004,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X32">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>30</v>
       </c>
@@ -2961,8 +3081,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X33">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>31</v>
       </c>
@@ -3034,8 +3158,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X34">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>32</v>
       </c>
@@ -3107,8 +3235,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X35">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>33</v>
       </c>
@@ -3180,8 +3312,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X36">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>34</v>
       </c>
@@ -3253,8 +3389,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X37">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>35</v>
       </c>
@@ -3326,8 +3466,12 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X38">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>36</v>
       </c>
@@ -3399,8 +3543,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X39">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>37</v>
       </c>
@@ -3472,8 +3620,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X40">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>38</v>
       </c>
@@ -3545,8 +3697,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X41">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>39</v>
       </c>
@@ -3618,8 +3774,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X42">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>40</v>
       </c>
@@ -3691,8 +3851,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X43">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>41</v>
       </c>
@@ -3764,8 +3928,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X44">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>42</v>
       </c>
@@ -3837,8 +4005,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X45">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>43</v>
       </c>
@@ -3910,8 +4082,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X46">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>44</v>
       </c>
@@ -3983,8 +4159,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X47">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>45</v>
       </c>
@@ -4056,8 +4236,12 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X48">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>46</v>
       </c>
@@ -4129,8 +4313,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X49">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>47</v>
       </c>
@@ -4202,8 +4390,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X50">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>48</v>
       </c>
@@ -4275,8 +4467,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X51">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>49</v>
       </c>
@@ -4348,8 +4544,12 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X52">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>50</v>
       </c>
@@ -4421,8 +4621,12 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X53">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>51</v>
       </c>
@@ -4494,8 +4698,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X54">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>52</v>
       </c>
@@ -4567,8 +4775,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X55">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>53</v>
       </c>
@@ -4640,8 +4852,12 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X56">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>54</v>
       </c>
@@ -4713,8 +4929,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X57">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>55</v>
       </c>
@@ -4786,8 +5006,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X58">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>56</v>
       </c>
@@ -4859,8 +5083,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X59">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>57</v>
       </c>
@@ -4932,8 +5160,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X60">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C61">
         <v>93.396551724137893</v>
       </c>
@@ -4942,79 +5174,79 @@
         <v>92.068965517241381</v>
       </c>
       <c r="E61">
-        <f t="shared" ref="E61:W61" si="2">AVERAGE(E3:E60)</f>
+        <f t="shared" ref="E61:W61" si="3">AVERAGE(E3:E60)</f>
         <v>92.793103448275858</v>
       </c>
       <c r="F61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>89.827586206896555</v>
       </c>
       <c r="G61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>89.965517241379317</v>
       </c>
       <c r="H61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>90.120689655172413</v>
       </c>
       <c r="I61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>89.965517241379317</v>
       </c>
       <c r="J61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>90.224137931034477</v>
       </c>
       <c r="K61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>88.775862068965523</v>
       </c>
       <c r="L61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>88.568965517241381</v>
       </c>
       <c r="M61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>87.810344827586206</v>
       </c>
       <c r="N61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>87.741379310344826</v>
       </c>
       <c r="O61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>87.465517241379317</v>
       </c>
       <c r="P61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>85.758620689655174</v>
       </c>
       <c r="Q61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>85.379310344827587</v>
       </c>
       <c r="R61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>86.879310344827587</v>
       </c>
       <c r="S61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>85.879310344827587</v>
       </c>
       <c r="T61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>84.15517241379311</v>
       </c>
       <c r="U61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>84.08620689655173</v>
       </c>
       <c r="V61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83.758620689655174</v>
       </c>
       <c r="W61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.31034482758620691</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add latest pipe count results
</commit_message>
<xml_diff>
--- a/src/Sandbox/Comparison.xlsx
+++ b/src/Sandbox/Comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joelv\Desktop\PumpjackPipeOptimizer\src\Sandbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3403C635-FD13-44FE-B1F7-2D4F5256B9D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D75A8D4-8713-4A57-A822-0145848B6BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F3EEF332-D963-44B3-89AD-4C5E1973BCE9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>FBE</t>
   </si>
@@ -162,6 +162,12 @@
   </si>
   <si>
     <t>Add FBE strategy</t>
+  </si>
+  <si>
+    <t>Bug fixes and perf</t>
+  </si>
+  <si>
+    <t>908a6d81fbc9a17161ab135f40d9dd8b2dd8787b</t>
   </si>
 </sst>
 </file>
@@ -557,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0EBF3A-B501-4205-AA83-0ECFC9C1E5B1}">
   <dimension ref="A1:X61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F31" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="W25" sqref="W25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,6 +638,9 @@
       <c r="V1" s="3" t="s">
         <v>41</v>
       </c>
+      <c r="W1" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="2" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -698,13 +707,16 @@
       <c r="V2" s="4" t="s">
         <v>40</v>
       </c>
+      <c r="W2" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
       <c r="B3">
-        <f>MIN(C3:V3)</f>
+        <f>MIN(C3:W3)</f>
         <v>16</v>
       </c>
       <c r="C3">
@@ -768,11 +780,10 @@
         <v>16</v>
       </c>
       <c r="W3">
+        <v>16</v>
+      </c>
+      <c r="X3">
         <f>V3-B3</f>
-        <v>0</v>
-      </c>
-      <c r="X3">
-        <f>D3-V3</f>
         <v>0</v>
       </c>
     </row>
@@ -781,7 +792,7 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B60" si="0">MIN(C4:V4)</f>
+        <f t="shared" ref="B4:B60" si="0">MIN(C4:W4)</f>
         <v>121</v>
       </c>
       <c r="C4">
@@ -845,12 +856,11 @@
         <v>121</v>
       </c>
       <c r="W4">
-        <f t="shared" ref="W4:W60" si="1">V4-B4</f>
+        <v>121</v>
+      </c>
+      <c r="X4">
+        <f t="shared" ref="X4:X60" si="1">V4-B4</f>
         <v>0</v>
-      </c>
-      <c r="X4">
-        <f t="shared" ref="X4:X60" si="2">D4-V4</f>
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -922,12 +932,11 @@
         <v>95</v>
       </c>
       <c r="W5">
+        <v>95</v>
+      </c>
+      <c r="X5">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X5">
-        <f t="shared" si="2"/>
-        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -999,12 +1008,11 @@
         <v>78</v>
       </c>
       <c r="W6">
+        <v>78</v>
+      </c>
+      <c r="X6">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X6">
-        <f t="shared" si="2"/>
-        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
@@ -1076,12 +1084,11 @@
         <v>82</v>
       </c>
       <c r="W7">
+        <v>83</v>
+      </c>
+      <c r="X7">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X7">
-        <f t="shared" si="2"/>
-        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
@@ -1153,12 +1160,11 @@
         <v>73</v>
       </c>
       <c r="W8">
+        <v>75</v>
+      </c>
+      <c r="X8">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X8">
-        <f t="shared" si="2"/>
-        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
@@ -1167,7 +1173,7 @@
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C9">
         <v>96</v>
@@ -1230,12 +1236,11 @@
         <v>90</v>
       </c>
       <c r="W9">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>89</v>
       </c>
       <c r="X9">
-        <f t="shared" si="2"/>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
@@ -1244,7 +1249,7 @@
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C10">
         <v>82</v>
@@ -1307,12 +1312,11 @@
         <v>66</v>
       </c>
       <c r="W10">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="X10">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
@@ -1384,12 +1388,11 @@
         <v>86</v>
       </c>
       <c r="W11">
+        <v>86</v>
+      </c>
+      <c r="X11">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X11">
-        <f t="shared" si="2"/>
-        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
@@ -1461,12 +1464,11 @@
         <v>103</v>
       </c>
       <c r="W12">
+        <v>103</v>
+      </c>
+      <c r="X12">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X12">
-        <f t="shared" si="2"/>
-        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
@@ -1538,12 +1540,11 @@
         <v>102</v>
       </c>
       <c r="W13">
+        <v>104</v>
+      </c>
+      <c r="X13">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X13">
-        <f t="shared" si="2"/>
-        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
@@ -1615,12 +1616,11 @@
         <v>54</v>
       </c>
       <c r="W14">
+        <v>54</v>
+      </c>
+      <c r="X14">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X14">
-        <f t="shared" si="2"/>
-        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
@@ -1692,12 +1692,11 @@
         <v>76</v>
       </c>
       <c r="W15">
+        <v>76</v>
+      </c>
+      <c r="X15">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X15">
-        <f t="shared" si="2"/>
-        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
@@ -1706,7 +1705,7 @@
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C16">
         <v>101</v>
@@ -1769,12 +1768,11 @@
         <v>92</v>
       </c>
       <c r="W16">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="X16">
-        <f t="shared" si="2"/>
-        <v>13</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
@@ -1846,12 +1844,11 @@
         <v>67</v>
       </c>
       <c r="W17">
+        <v>67</v>
+      </c>
+      <c r="X17">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X17">
-        <f t="shared" si="2"/>
-        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
@@ -1923,12 +1920,11 @@
         <v>82</v>
       </c>
       <c r="W18">
+        <v>80</v>
+      </c>
+      <c r="X18">
         <f t="shared" si="1"/>
         <v>2</v>
-      </c>
-      <c r="X18">
-        <f t="shared" si="2"/>
-        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
@@ -2000,12 +1996,11 @@
         <v>28</v>
       </c>
       <c r="W19">
+        <v>28</v>
+      </c>
+      <c r="X19">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X19">
-        <f t="shared" si="2"/>
-        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
@@ -2077,11 +2072,10 @@
         <v>37</v>
       </c>
       <c r="W20">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="X20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2154,12 +2148,11 @@
         <v>31</v>
       </c>
       <c r="W21">
+        <v>31</v>
+      </c>
+      <c r="X21">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X21">
-        <f t="shared" si="2"/>
-        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
@@ -2168,7 +2161,7 @@
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22">
         <v>48</v>
@@ -2231,11 +2224,10 @@
         <v>49</v>
       </c>
       <c r="W22">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="X22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -2308,11 +2300,10 @@
         <v>14</v>
       </c>
       <c r="W23">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="X23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2322,7 +2313,7 @@
       </c>
       <c r="B24">
         <f t="shared" si="0"/>
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C24">
         <v>65</v>
@@ -2385,12 +2376,11 @@
         <v>57</v>
       </c>
       <c r="W24">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="X24">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
@@ -2462,12 +2452,11 @@
         <v>67</v>
       </c>
       <c r="W25">
+        <v>67</v>
+      </c>
+      <c r="X25">
         <f t="shared" si="1"/>
         <v>4</v>
-      </c>
-      <c r="X25">
-        <f t="shared" si="2"/>
-        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
@@ -2539,11 +2528,10 @@
         <v>29</v>
       </c>
       <c r="W26">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="X26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2616,11 +2604,10 @@
         <v>29</v>
       </c>
       <c r="W27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="X27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2693,12 +2680,11 @@
         <v>66</v>
       </c>
       <c r="W28">
+        <v>67</v>
+      </c>
+      <c r="X28">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X28">
-        <f t="shared" si="2"/>
-        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
@@ -2770,11 +2756,10 @@
         <v>46</v>
       </c>
       <c r="W29">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="X29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2847,12 +2832,11 @@
         <v>44</v>
       </c>
       <c r="W30">
+        <v>44</v>
+      </c>
+      <c r="X30">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X30">
-        <f t="shared" si="2"/>
-        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
@@ -2924,12 +2908,11 @@
         <v>84</v>
       </c>
       <c r="W31">
+        <v>84</v>
+      </c>
+      <c r="X31">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X31">
-        <f t="shared" si="2"/>
-        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
@@ -2938,7 +2921,7 @@
       </c>
       <c r="B32">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C32">
         <v>70</v>
@@ -3001,12 +2984,11 @@
         <v>58</v>
       </c>
       <c r="W32">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="X32">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.25">
@@ -3078,12 +3060,11 @@
         <v>71</v>
       </c>
       <c r="W33">
+        <v>71</v>
+      </c>
+      <c r="X33">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X33">
-        <f t="shared" si="2"/>
-        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.25">
@@ -3155,12 +3136,11 @@
         <v>55</v>
       </c>
       <c r="W34">
+        <v>57</v>
+      </c>
+      <c r="X34">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X34">
-        <f t="shared" si="2"/>
-        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.25">
@@ -3232,12 +3212,11 @@
         <v>44</v>
       </c>
       <c r="W35">
+        <v>44</v>
+      </c>
+      <c r="X35">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X35">
-        <f t="shared" si="2"/>
-        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
@@ -3309,12 +3288,11 @@
         <v>127</v>
       </c>
       <c r="W36">
+        <v>127</v>
+      </c>
+      <c r="X36">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X36">
-        <f t="shared" si="2"/>
-        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.25">
@@ -3386,12 +3364,11 @@
         <v>134</v>
       </c>
       <c r="W37">
+        <v>134</v>
+      </c>
+      <c r="X37">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X37">
-        <f t="shared" si="2"/>
-        <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.25">
@@ -3463,12 +3440,11 @@
         <v>76</v>
       </c>
       <c r="W38">
+        <v>80</v>
+      </c>
+      <c r="X38">
         <f t="shared" si="1"/>
         <v>2</v>
-      </c>
-      <c r="X38">
-        <f t="shared" si="2"/>
-        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.25">
@@ -3540,12 +3516,11 @@
         <v>91</v>
       </c>
       <c r="W39">
+        <v>91</v>
+      </c>
+      <c r="X39">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X39">
-        <f t="shared" si="2"/>
-        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.25">
@@ -3617,12 +3592,11 @@
         <v>88</v>
       </c>
       <c r="W40">
+        <v>88</v>
+      </c>
+      <c r="X40">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X40">
-        <f t="shared" si="2"/>
-        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.25">
@@ -3694,12 +3668,11 @@
         <v>78</v>
       </c>
       <c r="W41">
+        <v>78</v>
+      </c>
+      <c r="X41">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X41">
-        <f t="shared" si="2"/>
-        <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.25">
@@ -3771,12 +3744,11 @@
         <v>87</v>
       </c>
       <c r="W42">
+        <v>87</v>
+      </c>
+      <c r="X42">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X42">
-        <f t="shared" si="2"/>
-        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.25">
@@ -3848,12 +3820,11 @@
         <v>114</v>
       </c>
       <c r="W43">
+        <v>114</v>
+      </c>
+      <c r="X43">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X43">
-        <f t="shared" si="2"/>
-        <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.25">
@@ -3925,11 +3896,10 @@
         <v>103</v>
       </c>
       <c r="W44">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>103</v>
       </c>
       <c r="X44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4002,12 +3972,11 @@
         <v>118</v>
       </c>
       <c r="W45">
+        <v>119</v>
+      </c>
+      <c r="X45">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X45">
-        <f t="shared" si="2"/>
-        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.25">
@@ -4079,12 +4048,11 @@
         <v>112</v>
       </c>
       <c r="W46">
+        <v>118</v>
+      </c>
+      <c r="X46">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X46">
-        <f t="shared" si="2"/>
-        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.25">
@@ -4156,12 +4124,11 @@
         <v>90</v>
       </c>
       <c r="W47">
+        <v>91</v>
+      </c>
+      <c r="X47">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X47">
-        <f t="shared" si="2"/>
-        <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.25">
@@ -4233,12 +4200,11 @@
         <v>115</v>
       </c>
       <c r="W48">
+        <v>111</v>
+      </c>
+      <c r="X48">
         <f t="shared" si="1"/>
         <v>4</v>
-      </c>
-      <c r="X48">
-        <f t="shared" si="2"/>
-        <v>33</v>
       </c>
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.25">
@@ -4310,12 +4276,11 @@
         <v>112</v>
       </c>
       <c r="W49">
+        <v>112</v>
+      </c>
+      <c r="X49">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X49">
-        <f t="shared" si="2"/>
-        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.25">
@@ -4387,12 +4352,11 @@
         <v>124</v>
       </c>
       <c r="W50">
+        <v>128</v>
+      </c>
+      <c r="X50">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X50">
-        <f t="shared" si="2"/>
-        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.25">
@@ -4464,12 +4428,11 @@
         <v>86</v>
       </c>
       <c r="W51">
+        <v>89</v>
+      </c>
+      <c r="X51">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X51">
-        <f t="shared" si="2"/>
-        <v>19</v>
       </c>
     </row>
     <row r="52" spans="1:24" x14ac:dyDescent="0.25">
@@ -4541,12 +4504,11 @@
         <v>123</v>
       </c>
       <c r="W52">
+        <v>123</v>
+      </c>
+      <c r="X52">
         <f t="shared" si="1"/>
         <v>1</v>
-      </c>
-      <c r="X52">
-        <f t="shared" si="2"/>
-        <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:24" x14ac:dyDescent="0.25">
@@ -4618,12 +4580,11 @@
         <v>119</v>
       </c>
       <c r="W53">
+        <v>118</v>
+      </c>
+      <c r="X53">
         <f t="shared" si="1"/>
         <v>1</v>
-      </c>
-      <c r="X53">
-        <f t="shared" si="2"/>
-        <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:24" x14ac:dyDescent="0.25">
@@ -4695,12 +4656,11 @@
         <v>167</v>
       </c>
       <c r="W54">
+        <v>168</v>
+      </c>
+      <c r="X54">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X54">
-        <f t="shared" si="2"/>
-        <v>18</v>
       </c>
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.25">
@@ -4772,12 +4732,11 @@
         <v>141</v>
       </c>
       <c r="W55">
+        <v>143</v>
+      </c>
+      <c r="X55">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X55">
-        <f t="shared" si="2"/>
-        <v>11</v>
       </c>
     </row>
     <row r="56" spans="1:24" x14ac:dyDescent="0.25">
@@ -4849,12 +4808,11 @@
         <v>103</v>
       </c>
       <c r="W56">
+        <v>101</v>
+      </c>
+      <c r="X56">
         <f t="shared" si="1"/>
         <v>2</v>
-      </c>
-      <c r="X56">
-        <f t="shared" si="2"/>
-        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.25">
@@ -4926,12 +4884,11 @@
         <v>110</v>
       </c>
       <c r="W57">
+        <v>112</v>
+      </c>
+      <c r="X57">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X57">
-        <f t="shared" si="2"/>
-        <v>13</v>
       </c>
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.25">
@@ -5003,12 +4960,11 @@
         <v>103</v>
       </c>
       <c r="W58">
+        <v>103</v>
+      </c>
+      <c r="X58">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X58">
-        <f t="shared" si="2"/>
-        <v>19</v>
       </c>
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.25">
@@ -5080,12 +5036,11 @@
         <v>114</v>
       </c>
       <c r="W59">
+        <v>114</v>
+      </c>
+      <c r="X59">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X59">
-        <f t="shared" si="2"/>
-        <v>28</v>
       </c>
     </row>
     <row r="60" spans="1:24" x14ac:dyDescent="0.25">
@@ -5157,12 +5112,11 @@
         <v>131</v>
       </c>
       <c r="W60">
+        <v>131</v>
+      </c>
+      <c r="X60">
         <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="X60">
-        <f t="shared" si="2"/>
-        <v>13</v>
       </c>
     </row>
     <row r="61" spans="1:24" x14ac:dyDescent="0.25">
@@ -5174,89 +5128,93 @@
         <v>92.068965517241381</v>
       </c>
       <c r="E61">
-        <f t="shared" ref="E61:W61" si="3">AVERAGE(E3:E60)</f>
+        <f t="shared" ref="E61:X61" si="2">AVERAGE(E3:E60)</f>
         <v>92.793103448275858</v>
       </c>
       <c r="F61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>89.827586206896555</v>
       </c>
       <c r="G61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>89.965517241379317</v>
       </c>
       <c r="H61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>90.120689655172413</v>
       </c>
       <c r="I61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>89.965517241379317</v>
       </c>
       <c r="J61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>90.224137931034477</v>
       </c>
       <c r="K61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>88.775862068965523</v>
       </c>
       <c r="L61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>88.568965517241381</v>
       </c>
       <c r="M61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>87.810344827586206</v>
       </c>
       <c r="N61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>87.741379310344826</v>
       </c>
       <c r="O61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>87.465517241379317</v>
       </c>
       <c r="P61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>85.758620689655174</v>
       </c>
       <c r="Q61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>85.379310344827587</v>
       </c>
       <c r="R61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>86.879310344827587</v>
       </c>
       <c r="S61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>85.879310344827587</v>
       </c>
       <c r="T61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>84.15517241379311</v>
       </c>
       <c r="U61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>84.08620689655173</v>
       </c>
       <c r="V61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>83.758620689655174</v>
       </c>
       <c r="W61">
-        <f t="shared" si="3"/>
-        <v>0.31034482758620691</v>
+        <f t="shared" si="2"/>
+        <v>83.948275862068968</v>
+      </c>
+      <c r="X61">
+        <f t="shared" si="2"/>
+        <v>0.48275862068965519</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:V60 C62:V1048576 C61:W61">
+  <conditionalFormatting sqref="C1:W60 C62:W1048576 C61:X61">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>INDIRECT(ADDRESS(ROW(), 2)) = INDIRECT(ADDRESS(ROW(), COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:V4">
+  <conditionalFormatting sqref="C4:W4">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>$B$3</formula>
     </cfRule>

</xml_diff>

<commit_message>
Add comparison for beacons
</commit_message>
<xml_diff>
--- a/src/Sandbox/Comparison.xlsx
+++ b/src/Sandbox/Comparison.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joelv\Desktop\PumpjackPipeOptimizer\src\Sandbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D75A8D4-8713-4A57-A822-0145848B6BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF585B37-2BA1-487D-96F0-C263771089E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F3EEF332-D963-44B3-89AD-4C5E1973BCE9}"/>
+    <workbookView xWindow="28680" yWindow="-210" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{F3EEF332-D963-44B3-89AD-4C5E1973BCE9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Pipes" sheetId="1" r:id="rId1"/>
+    <sheet name="Beacons" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
   <si>
     <t>FBE</t>
   </si>
@@ -169,6 +170,30 @@
   <si>
     <t>908a6d81fbc9a17161ab135f40d9dd8b2dd8787b</t>
   </si>
+  <si>
+    <t>Pipes</t>
+  </si>
+  <si>
+    <t>Poles</t>
+  </si>
+  <si>
+    <t>Beacons</t>
+  </si>
+  <si>
+    <t>FBE Pipes and Beacons</t>
+  </si>
+  <si>
+    <t>Best of Pipes and Joel's Beacons</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Best of Pipes and Beacons</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
 </sst>
 </file>
 
@@ -191,15 +216,39 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -216,21 +265,111 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <u/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <u/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -248,6 +387,27 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -563,8 +723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0EBF3A-B501-4205-AA83-0ECFC9C1E5B1}">
   <dimension ref="A1:X61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="W25" sqref="W25"/>
+    <sheetView topLeftCell="C27" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5210,13 +5370,2719 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:W60 C62:W1048576 C61:X61">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>INDIRECT(ADDRESS(ROW(), 2)) = INDIRECT(ADDRESS(ROW(), COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:W4">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>$B$3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A12EC30C-8E8D-4877-B5C6-99DE54BA8416}">
+  <dimension ref="A1:Q61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.7109375" style="13"/>
+    <col min="3" max="3" width="9.7109375" style="6"/>
+    <col min="4" max="4" width="9.7109375" style="7"/>
+    <col min="5" max="5" width="9.7109375" style="11"/>
+    <col min="6" max="6" width="9.7109375" style="6"/>
+    <col min="7" max="7" width="9.7109375" style="7"/>
+    <col min="8" max="8" width="9.7109375" style="11"/>
+    <col min="9" max="9" width="9.7109375" style="6"/>
+    <col min="10" max="10" width="9.7109375" style="7"/>
+    <col min="11" max="11" width="9.7109375" style="13"/>
+    <col min="12" max="12" width="9.7109375" style="6"/>
+    <col min="13" max="13" width="9.7109375" style="7"/>
+    <col min="14" max="14" width="9.7109375" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B1" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" s="13">
+        <f>MIN(E3,H3,K3)</f>
+        <v>5</v>
+      </c>
+      <c r="C3" s="6">
+        <f>MIN(F3,I3,L3)</f>
+        <v>7</v>
+      </c>
+      <c r="D3" s="7">
+        <f>MAX(G3,J3,M3)</f>
+        <v>22</v>
+      </c>
+      <c r="E3" s="11">
+        <v>5</v>
+      </c>
+      <c r="F3" s="6">
+        <v>7</v>
+      </c>
+      <c r="G3" s="7">
+        <v>22</v>
+      </c>
+      <c r="H3" s="11">
+        <v>5</v>
+      </c>
+      <c r="I3" s="6">
+        <v>8</v>
+      </c>
+      <c r="J3" s="7">
+        <v>22</v>
+      </c>
+      <c r="K3" s="13">
+        <v>5</v>
+      </c>
+      <c r="L3" s="6">
+        <v>8</v>
+      </c>
+      <c r="M3" s="7">
+        <v>22</v>
+      </c>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="13">
+        <f>MIN(E4,H4,K4)</f>
+        <v>70</v>
+      </c>
+      <c r="C4" s="6">
+        <f>MIN(F4,I4,L4)</f>
+        <v>33</v>
+      </c>
+      <c r="D4" s="7">
+        <f>MAX(G4,J4,M4)</f>
+        <v>105</v>
+      </c>
+      <c r="E4" s="11">
+        <v>76</v>
+      </c>
+      <c r="F4" s="6">
+        <v>33</v>
+      </c>
+      <c r="G4" s="7">
+        <v>105</v>
+      </c>
+      <c r="H4" s="11">
+        <v>70</v>
+      </c>
+      <c r="I4" s="6">
+        <v>36</v>
+      </c>
+      <c r="J4" s="7">
+        <v>103</v>
+      </c>
+      <c r="K4" s="13">
+        <v>70</v>
+      </c>
+      <c r="L4" s="6">
+        <v>33</v>
+      </c>
+      <c r="M4" s="7">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="13">
+        <f>MIN(E5,H5,K5)</f>
+        <v>40</v>
+      </c>
+      <c r="C5" s="6">
+        <f>MIN(F5,I5,L5)</f>
+        <v>28</v>
+      </c>
+      <c r="D5" s="7">
+        <f>MAX(G5,J5,M5)</f>
+        <v>84</v>
+      </c>
+      <c r="E5" s="11">
+        <v>48</v>
+      </c>
+      <c r="F5" s="6">
+        <v>30</v>
+      </c>
+      <c r="G5" s="7">
+        <v>79</v>
+      </c>
+      <c r="H5" s="11">
+        <v>40</v>
+      </c>
+      <c r="I5" s="6">
+        <v>28</v>
+      </c>
+      <c r="J5" s="7">
+        <v>80</v>
+      </c>
+      <c r="K5" s="13">
+        <v>40</v>
+      </c>
+      <c r="L5" s="6">
+        <v>28</v>
+      </c>
+      <c r="M5" s="7">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="13">
+        <f>MIN(E6,H6,K6)</f>
+        <v>43</v>
+      </c>
+      <c r="C6" s="6">
+        <f>MIN(F6,I6,L6)</f>
+        <v>18</v>
+      </c>
+      <c r="D6" s="7">
+        <f>MAX(G6,J6,M6)</f>
+        <v>60</v>
+      </c>
+      <c r="E6" s="11">
+        <v>44</v>
+      </c>
+      <c r="F6" s="6">
+        <v>21</v>
+      </c>
+      <c r="G6" s="7">
+        <v>60</v>
+      </c>
+      <c r="H6" s="11">
+        <v>43</v>
+      </c>
+      <c r="I6" s="6">
+        <v>18</v>
+      </c>
+      <c r="J6" s="7">
+        <v>54</v>
+      </c>
+      <c r="K6" s="13">
+        <v>43</v>
+      </c>
+      <c r="L6" s="6">
+        <v>22</v>
+      </c>
+      <c r="M6" s="7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="13">
+        <f>MIN(E7,H7,K7)</f>
+        <v>41</v>
+      </c>
+      <c r="C7" s="6">
+        <f>MIN(F7,I7,L7)</f>
+        <v>21</v>
+      </c>
+      <c r="D7" s="7">
+        <f>MAX(G7,J7,M7)</f>
+        <v>73</v>
+      </c>
+      <c r="E7" s="11">
+        <v>41</v>
+      </c>
+      <c r="F7" s="6">
+        <v>26</v>
+      </c>
+      <c r="G7" s="7">
+        <v>72</v>
+      </c>
+      <c r="H7" s="11">
+        <v>44</v>
+      </c>
+      <c r="I7" s="6">
+        <v>21</v>
+      </c>
+      <c r="J7" s="7">
+        <v>73</v>
+      </c>
+      <c r="K7" s="13">
+        <v>44</v>
+      </c>
+      <c r="L7" s="6">
+        <v>21</v>
+      </c>
+      <c r="M7" s="7">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" s="13">
+        <f>MIN(E8,H8,K8)</f>
+        <v>41</v>
+      </c>
+      <c r="C8" s="6">
+        <f>MIN(F8,I8,L8)</f>
+        <v>23</v>
+      </c>
+      <c r="D8" s="7">
+        <f>MAX(G8,J8,M8)</f>
+        <v>78</v>
+      </c>
+      <c r="E8" s="11">
+        <v>43</v>
+      </c>
+      <c r="F8" s="6">
+        <v>23</v>
+      </c>
+      <c r="G8" s="7">
+        <v>76</v>
+      </c>
+      <c r="H8" s="11">
+        <v>41</v>
+      </c>
+      <c r="I8" s="6">
+        <v>24</v>
+      </c>
+      <c r="J8" s="7">
+        <v>78</v>
+      </c>
+      <c r="K8" s="13">
+        <v>41</v>
+      </c>
+      <c r="L8" s="6">
+        <v>24</v>
+      </c>
+      <c r="M8" s="7">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="13">
+        <f>MIN(E9,H9,K9)</f>
+        <v>50</v>
+      </c>
+      <c r="C9" s="6">
+        <f>MIN(F9,I9,L9)</f>
+        <v>25</v>
+      </c>
+      <c r="D9" s="7">
+        <f>MAX(G9,J9,M9)</f>
+        <v>82</v>
+      </c>
+      <c r="E9" s="11">
+        <v>50</v>
+      </c>
+      <c r="F9" s="6">
+        <v>25</v>
+      </c>
+      <c r="G9" s="7">
+        <v>82</v>
+      </c>
+      <c r="H9" s="11">
+        <v>50</v>
+      </c>
+      <c r="I9" s="6">
+        <v>26</v>
+      </c>
+      <c r="J9" s="7">
+        <v>80</v>
+      </c>
+      <c r="K9" s="13">
+        <v>50</v>
+      </c>
+      <c r="L9" s="6">
+        <v>25</v>
+      </c>
+      <c r="M9" s="7">
+        <v>82</v>
+      </c>
+      <c r="Q9" s="17"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" s="13">
+        <f>MIN(E10,H10,K10)</f>
+        <v>31</v>
+      </c>
+      <c r="C10" s="6">
+        <f>MIN(F10,I10,L10)</f>
+        <v>20</v>
+      </c>
+      <c r="D10" s="7">
+        <f>MAX(G10,J10,M10)</f>
+        <v>62</v>
+      </c>
+      <c r="E10" s="11">
+        <v>31</v>
+      </c>
+      <c r="F10" s="6">
+        <v>21</v>
+      </c>
+      <c r="G10" s="7">
+        <v>58</v>
+      </c>
+      <c r="H10" s="11">
+        <v>35</v>
+      </c>
+      <c r="I10" s="6">
+        <v>20</v>
+      </c>
+      <c r="J10" s="7">
+        <v>62</v>
+      </c>
+      <c r="K10" s="13">
+        <v>35</v>
+      </c>
+      <c r="L10" s="6">
+        <v>20</v>
+      </c>
+      <c r="M10" s="7">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" s="13">
+        <f>MIN(E11,H11,K11)</f>
+        <v>40</v>
+      </c>
+      <c r="C11" s="6">
+        <f>MIN(F11,I11,L11)</f>
+        <v>24</v>
+      </c>
+      <c r="D11" s="7">
+        <f>MAX(G11,J11,M11)</f>
+        <v>75</v>
+      </c>
+      <c r="E11" s="11">
+        <v>40</v>
+      </c>
+      <c r="F11" s="6">
+        <v>24</v>
+      </c>
+      <c r="G11" s="7">
+        <v>75</v>
+      </c>
+      <c r="H11" s="11">
+        <v>41</v>
+      </c>
+      <c r="I11" s="6">
+        <v>24</v>
+      </c>
+      <c r="J11" s="7">
+        <v>73</v>
+      </c>
+      <c r="K11" s="13">
+        <v>41</v>
+      </c>
+      <c r="L11" s="6">
+        <v>24</v>
+      </c>
+      <c r="M11" s="7">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" s="13">
+        <f>MIN(E12,H12,K12)</f>
+        <v>36</v>
+      </c>
+      <c r="C12" s="6">
+        <f>MIN(F12,I12,L12)</f>
+        <v>30</v>
+      </c>
+      <c r="D12" s="7">
+        <f>MAX(G12,J12,M12)</f>
+        <v>85</v>
+      </c>
+      <c r="E12" s="11">
+        <v>40</v>
+      </c>
+      <c r="F12" s="6">
+        <v>31</v>
+      </c>
+      <c r="G12" s="7">
+        <v>84</v>
+      </c>
+      <c r="H12" s="11">
+        <v>36</v>
+      </c>
+      <c r="I12" s="6">
+        <v>30</v>
+      </c>
+      <c r="J12" s="7">
+        <v>85</v>
+      </c>
+      <c r="K12" s="13">
+        <v>36</v>
+      </c>
+      <c r="L12" s="6">
+        <v>30</v>
+      </c>
+      <c r="M12" s="7">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" s="13">
+        <f>MIN(E13,H13,K13)</f>
+        <v>43</v>
+      </c>
+      <c r="C13" s="6">
+        <f>MIN(F13,I13,L13)</f>
+        <v>29</v>
+      </c>
+      <c r="D13" s="7">
+        <f>MAX(G13,J13,M13)</f>
+        <v>84</v>
+      </c>
+      <c r="E13" s="11">
+        <v>45</v>
+      </c>
+      <c r="F13" s="6">
+        <v>30</v>
+      </c>
+      <c r="G13" s="7">
+        <v>84</v>
+      </c>
+      <c r="H13" s="11">
+        <v>43</v>
+      </c>
+      <c r="I13" s="6">
+        <v>29</v>
+      </c>
+      <c r="J13" s="7">
+        <v>82</v>
+      </c>
+      <c r="K13" s="13">
+        <v>43</v>
+      </c>
+      <c r="L13" s="6">
+        <v>29</v>
+      </c>
+      <c r="M13" s="7">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" s="13">
+        <f>MIN(E14,H14,K14)</f>
+        <v>29</v>
+      </c>
+      <c r="C14" s="6">
+        <f>MIN(F14,I14,L14)</f>
+        <v>17</v>
+      </c>
+      <c r="D14" s="7">
+        <f>MAX(G14,J14,M14)</f>
+        <v>54</v>
+      </c>
+      <c r="E14" s="11">
+        <v>35</v>
+      </c>
+      <c r="F14" s="6">
+        <v>19</v>
+      </c>
+      <c r="G14" s="7">
+        <v>54</v>
+      </c>
+      <c r="H14" s="11">
+        <v>29</v>
+      </c>
+      <c r="I14" s="6">
+        <v>17</v>
+      </c>
+      <c r="J14" s="7">
+        <v>53</v>
+      </c>
+      <c r="K14" s="13">
+        <v>29</v>
+      </c>
+      <c r="L14" s="6">
+        <v>17</v>
+      </c>
+      <c r="M14" s="7">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" s="13">
+        <f>MIN(E15,H15,K15)</f>
+        <v>32</v>
+      </c>
+      <c r="C15" s="6">
+        <f>MIN(F15,I15,L15)</f>
+        <v>22</v>
+      </c>
+      <c r="D15" s="7">
+        <f>MAX(G15,J15,M15)</f>
+        <v>69</v>
+      </c>
+      <c r="E15" s="11">
+        <v>42</v>
+      </c>
+      <c r="F15" s="6">
+        <v>24</v>
+      </c>
+      <c r="G15" s="7">
+        <v>67</v>
+      </c>
+      <c r="H15" s="11">
+        <v>32</v>
+      </c>
+      <c r="I15" s="6">
+        <v>22</v>
+      </c>
+      <c r="J15" s="7">
+        <v>67</v>
+      </c>
+      <c r="K15" s="13">
+        <v>32</v>
+      </c>
+      <c r="L15" s="6">
+        <v>23</v>
+      </c>
+      <c r="M15" s="7">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" s="13">
+        <f>MIN(E16,H16,K16)</f>
+        <v>39</v>
+      </c>
+      <c r="C16" s="6">
+        <f>MIN(F16,I16,L16)</f>
+        <v>22</v>
+      </c>
+      <c r="D16" s="7">
+        <f>MAX(G16,J16,M16)</f>
+        <v>73</v>
+      </c>
+      <c r="E16" s="11">
+        <v>39</v>
+      </c>
+      <c r="F16" s="6">
+        <v>24</v>
+      </c>
+      <c r="G16" s="7">
+        <v>70</v>
+      </c>
+      <c r="H16" s="11">
+        <v>40</v>
+      </c>
+      <c r="I16" s="6">
+        <v>22</v>
+      </c>
+      <c r="J16" s="7">
+        <v>69</v>
+      </c>
+      <c r="K16" s="13">
+        <v>40</v>
+      </c>
+      <c r="L16" s="6">
+        <v>24</v>
+      </c>
+      <c r="M16" s="7">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17" s="13">
+        <f>MIN(E17,H17,K17)</f>
+        <v>35</v>
+      </c>
+      <c r="C17" s="6">
+        <f>MIN(F17,I17,L17)</f>
+        <v>21</v>
+      </c>
+      <c r="D17" s="7">
+        <f>MAX(G17,J17,M17)</f>
+        <v>69</v>
+      </c>
+      <c r="E17" s="11">
+        <v>35</v>
+      </c>
+      <c r="F17" s="6">
+        <v>21</v>
+      </c>
+      <c r="G17" s="7">
+        <v>65</v>
+      </c>
+      <c r="H17" s="11">
+        <v>35</v>
+      </c>
+      <c r="I17" s="6">
+        <v>23</v>
+      </c>
+      <c r="J17" s="7">
+        <v>69</v>
+      </c>
+      <c r="K17" s="13">
+        <v>35</v>
+      </c>
+      <c r="L17" s="6">
+        <v>23</v>
+      </c>
+      <c r="M17" s="7">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18" s="13">
+        <f>MIN(E18,H18,K18)</f>
+        <v>41</v>
+      </c>
+      <c r="C18" s="6">
+        <f>MIN(F18,I18,L18)</f>
+        <v>23</v>
+      </c>
+      <c r="D18" s="7">
+        <f>MAX(G18,J18,M18)</f>
+        <v>67</v>
+      </c>
+      <c r="E18" s="11">
+        <v>42</v>
+      </c>
+      <c r="F18" s="6">
+        <v>23</v>
+      </c>
+      <c r="G18" s="7">
+        <v>67</v>
+      </c>
+      <c r="H18" s="11">
+        <v>41</v>
+      </c>
+      <c r="I18" s="6">
+        <v>24</v>
+      </c>
+      <c r="J18" s="7">
+        <v>66</v>
+      </c>
+      <c r="K18" s="13">
+        <v>41</v>
+      </c>
+      <c r="L18" s="6">
+        <v>24</v>
+      </c>
+      <c r="M18" s="7">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19" s="13">
+        <f>MIN(E19,H19,K19)</f>
+        <v>14</v>
+      </c>
+      <c r="C19" s="6">
+        <f>MIN(F19,I19,L19)</f>
+        <v>12</v>
+      </c>
+      <c r="D19" s="7">
+        <f>MAX(G19,J19,M19)</f>
+        <v>38</v>
+      </c>
+      <c r="E19" s="11">
+        <v>15</v>
+      </c>
+      <c r="F19" s="6">
+        <v>13</v>
+      </c>
+      <c r="G19" s="7">
+        <v>38</v>
+      </c>
+      <c r="H19" s="11">
+        <v>14</v>
+      </c>
+      <c r="I19" s="6">
+        <v>12</v>
+      </c>
+      <c r="J19" s="7">
+        <v>36</v>
+      </c>
+      <c r="K19" s="13">
+        <v>14</v>
+      </c>
+      <c r="L19" s="6">
+        <v>12</v>
+      </c>
+      <c r="M19" s="7">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20" s="13">
+        <f>MIN(E20,H20,K20)</f>
+        <v>17</v>
+      </c>
+      <c r="C20" s="6">
+        <f>MIN(F20,I20,L20)</f>
+        <v>12</v>
+      </c>
+      <c r="D20" s="7">
+        <f>MAX(G20,J20,M20)</f>
+        <v>45</v>
+      </c>
+      <c r="E20" s="11">
+        <v>17</v>
+      </c>
+      <c r="F20" s="6">
+        <v>13</v>
+      </c>
+      <c r="G20" s="7">
+        <v>45</v>
+      </c>
+      <c r="H20" s="11">
+        <v>17</v>
+      </c>
+      <c r="I20" s="6">
+        <v>12</v>
+      </c>
+      <c r="J20" s="7">
+        <v>45</v>
+      </c>
+      <c r="K20" s="13">
+        <v>17</v>
+      </c>
+      <c r="L20" s="6">
+        <v>12</v>
+      </c>
+      <c r="M20" s="7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21" s="13">
+        <f>MIN(E21,H21,K21)</f>
+        <v>14</v>
+      </c>
+      <c r="C21" s="6">
+        <f>MIN(F21,I21,L21)</f>
+        <v>9</v>
+      </c>
+      <c r="D21" s="7">
+        <f>MAX(G21,J21,M21)</f>
+        <v>41</v>
+      </c>
+      <c r="E21" s="11">
+        <v>17</v>
+      </c>
+      <c r="F21" s="6">
+        <v>13</v>
+      </c>
+      <c r="G21" s="7">
+        <v>41</v>
+      </c>
+      <c r="H21" s="11">
+        <v>14</v>
+      </c>
+      <c r="I21" s="6">
+        <v>9</v>
+      </c>
+      <c r="J21" s="7">
+        <v>32</v>
+      </c>
+      <c r="K21" s="13">
+        <v>14</v>
+      </c>
+      <c r="L21" s="6">
+        <v>14</v>
+      </c>
+      <c r="M21" s="7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22" s="13">
+        <f>MIN(E22,H22,K22)</f>
+        <v>20</v>
+      </c>
+      <c r="C22" s="6">
+        <f>MIN(F22,I22,L22)</f>
+        <v>16</v>
+      </c>
+      <c r="D22" s="7">
+        <f>MAX(G22,J22,M22)</f>
+        <v>51</v>
+      </c>
+      <c r="E22" s="11">
+        <v>21</v>
+      </c>
+      <c r="F22" s="6">
+        <v>16</v>
+      </c>
+      <c r="G22" s="7">
+        <v>50</v>
+      </c>
+      <c r="H22" s="11">
+        <v>20</v>
+      </c>
+      <c r="I22" s="6">
+        <v>17</v>
+      </c>
+      <c r="J22" s="7">
+        <v>50</v>
+      </c>
+      <c r="K22" s="13">
+        <v>20</v>
+      </c>
+      <c r="L22" s="6">
+        <v>16</v>
+      </c>
+      <c r="M22" s="7">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23" s="13">
+        <f>MIN(E23,H23,K23)</f>
+        <v>8</v>
+      </c>
+      <c r="C23" s="6">
+        <f>MIN(F23,I23,L23)</f>
+        <v>7</v>
+      </c>
+      <c r="D23" s="7">
+        <f>MAX(G23,J23,M23)</f>
+        <v>25</v>
+      </c>
+      <c r="E23" s="11">
+        <v>8</v>
+      </c>
+      <c r="F23" s="6">
+        <v>8</v>
+      </c>
+      <c r="G23" s="7">
+        <v>25</v>
+      </c>
+      <c r="H23" s="11">
+        <v>8</v>
+      </c>
+      <c r="I23" s="6">
+        <v>7</v>
+      </c>
+      <c r="J23" s="7">
+        <v>22</v>
+      </c>
+      <c r="K23" s="13">
+        <v>8</v>
+      </c>
+      <c r="L23" s="6">
+        <v>9</v>
+      </c>
+      <c r="M23" s="7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24" s="13">
+        <f>MIN(E24,H24,K24)</f>
+        <v>28</v>
+      </c>
+      <c r="C24" s="6">
+        <f>MIN(F24,I24,L24)</f>
+        <v>18</v>
+      </c>
+      <c r="D24" s="7">
+        <f>MAX(G24,J24,M24)</f>
+        <v>64</v>
+      </c>
+      <c r="E24" s="11">
+        <v>28</v>
+      </c>
+      <c r="F24" s="6">
+        <v>18</v>
+      </c>
+      <c r="G24" s="7">
+        <v>64</v>
+      </c>
+      <c r="H24" s="11">
+        <v>28</v>
+      </c>
+      <c r="I24" s="6">
+        <v>19</v>
+      </c>
+      <c r="J24" s="7">
+        <v>62</v>
+      </c>
+      <c r="K24" s="13">
+        <v>28</v>
+      </c>
+      <c r="L24" s="6">
+        <v>19</v>
+      </c>
+      <c r="M24" s="7">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25" s="13">
+        <f>MIN(E25,H25,K25)</f>
+        <v>31</v>
+      </c>
+      <c r="C25" s="6">
+        <f>MIN(F25,I25,L25)</f>
+        <v>23</v>
+      </c>
+      <c r="D25" s="7">
+        <f>MAX(G25,J25,M25)</f>
+        <v>62</v>
+      </c>
+      <c r="E25" s="11">
+        <v>32</v>
+      </c>
+      <c r="F25" s="6">
+        <v>23</v>
+      </c>
+      <c r="G25" s="7">
+        <v>62</v>
+      </c>
+      <c r="H25" s="11">
+        <v>31</v>
+      </c>
+      <c r="I25" s="6">
+        <v>23</v>
+      </c>
+      <c r="J25" s="7">
+        <v>60</v>
+      </c>
+      <c r="K25" s="13">
+        <v>31</v>
+      </c>
+      <c r="L25" s="6">
+        <v>23</v>
+      </c>
+      <c r="M25" s="7">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26" s="13">
+        <f>MIN(E26,H26,K26)</f>
+        <v>11</v>
+      </c>
+      <c r="C26" s="6">
+        <f>MIN(F26,I26,L26)</f>
+        <v>9</v>
+      </c>
+      <c r="D26" s="7">
+        <f>MAX(G26,J26,M26)</f>
+        <v>30</v>
+      </c>
+      <c r="E26" s="11">
+        <v>11</v>
+      </c>
+      <c r="F26" s="6">
+        <v>9</v>
+      </c>
+      <c r="G26" s="7">
+        <v>29</v>
+      </c>
+      <c r="H26" s="11">
+        <v>11</v>
+      </c>
+      <c r="I26" s="6">
+        <v>9</v>
+      </c>
+      <c r="J26" s="7">
+        <v>30</v>
+      </c>
+      <c r="K26" s="13">
+        <v>11</v>
+      </c>
+      <c r="L26" s="6">
+        <v>9</v>
+      </c>
+      <c r="M26" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>24</v>
+      </c>
+      <c r="B27" s="13">
+        <f>MIN(E27,H27,K27)</f>
+        <v>13</v>
+      </c>
+      <c r="C27" s="6">
+        <f>MIN(F27,I27,L27)</f>
+        <v>9</v>
+      </c>
+      <c r="D27" s="7">
+        <f>MAX(G27,J27,M27)</f>
+        <v>28</v>
+      </c>
+      <c r="E27" s="11">
+        <v>13</v>
+      </c>
+      <c r="F27" s="6">
+        <v>10</v>
+      </c>
+      <c r="G27" s="7">
+        <v>28</v>
+      </c>
+      <c r="H27" s="11">
+        <v>13</v>
+      </c>
+      <c r="I27" s="6">
+        <v>9</v>
+      </c>
+      <c r="J27" s="7">
+        <v>28</v>
+      </c>
+      <c r="K27" s="13">
+        <v>13</v>
+      </c>
+      <c r="L27" s="6">
+        <v>9</v>
+      </c>
+      <c r="M27" s="7">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>25</v>
+      </c>
+      <c r="B28" s="13">
+        <f>MIN(E28,H28,K28)</f>
+        <v>29</v>
+      </c>
+      <c r="C28" s="6">
+        <f>MIN(F28,I28,L28)</f>
+        <v>17</v>
+      </c>
+      <c r="D28" s="7">
+        <f>MAX(G28,J28,M28)</f>
+        <v>56</v>
+      </c>
+      <c r="E28" s="11">
+        <v>29</v>
+      </c>
+      <c r="F28" s="6">
+        <v>17</v>
+      </c>
+      <c r="G28" s="7">
+        <v>56</v>
+      </c>
+      <c r="H28" s="11">
+        <v>33</v>
+      </c>
+      <c r="I28" s="6">
+        <v>19</v>
+      </c>
+      <c r="J28" s="7">
+        <v>56</v>
+      </c>
+      <c r="K28" s="13">
+        <v>33</v>
+      </c>
+      <c r="L28" s="6">
+        <v>19</v>
+      </c>
+      <c r="M28" s="7">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>26</v>
+      </c>
+      <c r="B29" s="13">
+        <f>MIN(E29,H29,K29)</f>
+        <v>26</v>
+      </c>
+      <c r="C29" s="6">
+        <f>MIN(F29,I29,L29)</f>
+        <v>15</v>
+      </c>
+      <c r="D29" s="7">
+        <f>MAX(G29,J29,M29)</f>
+        <v>47</v>
+      </c>
+      <c r="E29" s="11">
+        <v>26</v>
+      </c>
+      <c r="F29" s="6">
+        <v>15</v>
+      </c>
+      <c r="G29" s="7">
+        <v>47</v>
+      </c>
+      <c r="H29" s="11">
+        <v>26</v>
+      </c>
+      <c r="I29" s="6">
+        <v>16</v>
+      </c>
+      <c r="J29" s="7">
+        <v>47</v>
+      </c>
+      <c r="K29" s="13">
+        <v>26</v>
+      </c>
+      <c r="L29" s="6">
+        <v>16</v>
+      </c>
+      <c r="M29" s="7">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>27</v>
+      </c>
+      <c r="B30" s="13">
+        <f>MIN(E30,H30,K30)</f>
+        <v>26</v>
+      </c>
+      <c r="C30" s="6">
+        <f>MIN(F30,I30,L30)</f>
+        <v>15</v>
+      </c>
+      <c r="D30" s="7">
+        <f>MAX(G30,J30,M30)</f>
+        <v>54</v>
+      </c>
+      <c r="E30" s="11">
+        <v>27</v>
+      </c>
+      <c r="F30" s="6">
+        <v>18</v>
+      </c>
+      <c r="G30" s="7">
+        <v>50</v>
+      </c>
+      <c r="H30" s="11">
+        <v>26</v>
+      </c>
+      <c r="I30" s="6">
+        <v>15</v>
+      </c>
+      <c r="J30" s="7">
+        <v>54</v>
+      </c>
+      <c r="K30" s="13">
+        <v>26</v>
+      </c>
+      <c r="L30" s="6">
+        <v>15</v>
+      </c>
+      <c r="M30" s="7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>28</v>
+      </c>
+      <c r="B31" s="13">
+        <f>MIN(E31,H31,K31)</f>
+        <v>38</v>
+      </c>
+      <c r="C31" s="6">
+        <f>MIN(F31,I31,L31)</f>
+        <v>21</v>
+      </c>
+      <c r="D31" s="7">
+        <f>MAX(G31,J31,M31)</f>
+        <v>72</v>
+      </c>
+      <c r="E31" s="11">
+        <v>39</v>
+      </c>
+      <c r="F31" s="6">
+        <v>22</v>
+      </c>
+      <c r="G31" s="7">
+        <v>72</v>
+      </c>
+      <c r="H31" s="11">
+        <v>38</v>
+      </c>
+      <c r="I31" s="6">
+        <v>21</v>
+      </c>
+      <c r="J31" s="7">
+        <v>66</v>
+      </c>
+      <c r="K31" s="13">
+        <v>38</v>
+      </c>
+      <c r="L31" s="6">
+        <v>21</v>
+      </c>
+      <c r="M31" s="7">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>29</v>
+      </c>
+      <c r="B32" s="13">
+        <f>MIN(E32,H32,K32)</f>
+        <v>30</v>
+      </c>
+      <c r="C32" s="6">
+        <f>MIN(F32,I32,L32)</f>
+        <v>18</v>
+      </c>
+      <c r="D32" s="7">
+        <f>MAX(G32,J32,M32)</f>
+        <v>53</v>
+      </c>
+      <c r="E32" s="11">
+        <v>33</v>
+      </c>
+      <c r="F32" s="6">
+        <v>20</v>
+      </c>
+      <c r="G32" s="7">
+        <v>53</v>
+      </c>
+      <c r="H32" s="11">
+        <v>30</v>
+      </c>
+      <c r="I32" s="6">
+        <v>18</v>
+      </c>
+      <c r="J32" s="7">
+        <v>51</v>
+      </c>
+      <c r="K32" s="13">
+        <v>30</v>
+      </c>
+      <c r="L32" s="6">
+        <v>18</v>
+      </c>
+      <c r="M32" s="7">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>30</v>
+      </c>
+      <c r="B33" s="13">
+        <f>MIN(E33,H33,K33)</f>
+        <v>30</v>
+      </c>
+      <c r="C33" s="6">
+        <f>MIN(F33,I33,L33)</f>
+        <v>19</v>
+      </c>
+      <c r="D33" s="7">
+        <f>MAX(G33,J33,M33)</f>
+        <v>69</v>
+      </c>
+      <c r="E33" s="11">
+        <v>30</v>
+      </c>
+      <c r="F33" s="6">
+        <v>23</v>
+      </c>
+      <c r="G33" s="7">
+        <v>68</v>
+      </c>
+      <c r="H33" s="11">
+        <v>34</v>
+      </c>
+      <c r="I33" s="6">
+        <v>19</v>
+      </c>
+      <c r="J33" s="7">
+        <v>68</v>
+      </c>
+      <c r="K33" s="13">
+        <v>34</v>
+      </c>
+      <c r="L33" s="6">
+        <v>24</v>
+      </c>
+      <c r="M33" s="7">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>31</v>
+      </c>
+      <c r="B34" s="13">
+        <f>MIN(E34,H34,K34)</f>
+        <v>27</v>
+      </c>
+      <c r="C34" s="6">
+        <f>MIN(F34,I34,L34)</f>
+        <v>21</v>
+      </c>
+      <c r="D34" s="7">
+        <f>MAX(G34,J34,M34)</f>
+        <v>61</v>
+      </c>
+      <c r="E34" s="11">
+        <v>29</v>
+      </c>
+      <c r="F34" s="6">
+        <v>21</v>
+      </c>
+      <c r="G34" s="7">
+        <v>61</v>
+      </c>
+      <c r="H34" s="11">
+        <v>27</v>
+      </c>
+      <c r="I34" s="6">
+        <v>21</v>
+      </c>
+      <c r="J34" s="7">
+        <v>58</v>
+      </c>
+      <c r="K34" s="13">
+        <v>27</v>
+      </c>
+      <c r="L34" s="6">
+        <v>21</v>
+      </c>
+      <c r="M34" s="7">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>32</v>
+      </c>
+      <c r="B35" s="13">
+        <f>MIN(E35,H35,K35)</f>
+        <v>19</v>
+      </c>
+      <c r="C35" s="6">
+        <f>MIN(F35,I35,L35)</f>
+        <v>14</v>
+      </c>
+      <c r="D35" s="7">
+        <f>MAX(G35,J35,M35)</f>
+        <v>50</v>
+      </c>
+      <c r="E35" s="11">
+        <v>20</v>
+      </c>
+      <c r="F35" s="6">
+        <v>15</v>
+      </c>
+      <c r="G35" s="7">
+        <v>48</v>
+      </c>
+      <c r="H35" s="11">
+        <v>19</v>
+      </c>
+      <c r="I35" s="6">
+        <v>14</v>
+      </c>
+      <c r="J35" s="7">
+        <v>50</v>
+      </c>
+      <c r="K35" s="13">
+        <v>19</v>
+      </c>
+      <c r="L35" s="6">
+        <v>14</v>
+      </c>
+      <c r="M35" s="7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>33</v>
+      </c>
+      <c r="B36" s="13">
+        <f>MIN(E36,H36,K36)</f>
+        <v>74</v>
+      </c>
+      <c r="C36" s="6">
+        <f>MIN(F36,I36,L36)</f>
+        <v>32</v>
+      </c>
+      <c r="D36" s="7">
+        <f>MAX(G36,J36,M36)</f>
+        <v>109</v>
+      </c>
+      <c r="E36" s="11">
+        <v>74</v>
+      </c>
+      <c r="F36" s="6">
+        <v>33</v>
+      </c>
+      <c r="G36" s="7">
+        <v>101</v>
+      </c>
+      <c r="H36" s="11">
+        <v>76</v>
+      </c>
+      <c r="I36" s="6">
+        <v>32</v>
+      </c>
+      <c r="J36" s="7">
+        <v>108</v>
+      </c>
+      <c r="K36" s="13">
+        <v>76</v>
+      </c>
+      <c r="L36" s="6">
+        <v>34</v>
+      </c>
+      <c r="M36" s="7">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>34</v>
+      </c>
+      <c r="B37" s="13">
+        <f>MIN(E37,H37,K37)</f>
+        <v>75</v>
+      </c>
+      <c r="C37" s="6">
+        <f>MIN(F37,I37,L37)</f>
+        <v>31</v>
+      </c>
+      <c r="D37" s="7">
+        <f>MAX(G37,J37,M37)</f>
+        <v>118</v>
+      </c>
+      <c r="E37" s="11">
+        <v>75</v>
+      </c>
+      <c r="F37" s="6">
+        <v>40</v>
+      </c>
+      <c r="G37" s="7">
+        <v>118</v>
+      </c>
+      <c r="H37" s="11">
+        <v>81</v>
+      </c>
+      <c r="I37" s="6">
+        <v>31</v>
+      </c>
+      <c r="J37" s="7">
+        <v>109</v>
+      </c>
+      <c r="K37" s="13">
+        <v>81</v>
+      </c>
+      <c r="L37" s="6">
+        <v>35</v>
+      </c>
+      <c r="M37" s="7">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>35</v>
+      </c>
+      <c r="B38" s="13">
+        <f>MIN(E38,H38,K38)</f>
+        <v>45</v>
+      </c>
+      <c r="C38" s="6">
+        <f>MIN(F38,I38,L38)</f>
+        <v>19</v>
+      </c>
+      <c r="D38" s="7">
+        <f>MAX(G38,J38,M38)</f>
+        <v>66</v>
+      </c>
+      <c r="E38" s="11">
+        <v>46</v>
+      </c>
+      <c r="F38" s="6">
+        <v>22</v>
+      </c>
+      <c r="G38" s="7">
+        <v>61</v>
+      </c>
+      <c r="H38" s="11">
+        <v>45</v>
+      </c>
+      <c r="I38" s="6">
+        <v>19</v>
+      </c>
+      <c r="J38" s="7">
+        <v>66</v>
+      </c>
+      <c r="K38" s="13">
+        <v>45</v>
+      </c>
+      <c r="L38" s="6">
+        <v>19</v>
+      </c>
+      <c r="M38" s="7">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>36</v>
+      </c>
+      <c r="B39" s="13">
+        <f>MIN(E39,H39,K39)</f>
+        <v>50</v>
+      </c>
+      <c r="C39" s="6">
+        <f>MIN(F39,I39,L39)</f>
+        <v>25</v>
+      </c>
+      <c r="D39" s="7">
+        <f>MAX(G39,J39,M39)</f>
+        <v>86</v>
+      </c>
+      <c r="E39" s="11">
+        <v>51</v>
+      </c>
+      <c r="F39" s="6">
+        <v>29</v>
+      </c>
+      <c r="G39" s="7">
+        <v>85</v>
+      </c>
+      <c r="H39" s="11">
+        <v>50</v>
+      </c>
+      <c r="I39" s="6">
+        <v>25</v>
+      </c>
+      <c r="J39" s="7">
+        <v>86</v>
+      </c>
+      <c r="K39" s="13">
+        <v>50</v>
+      </c>
+      <c r="L39" s="6">
+        <v>25</v>
+      </c>
+      <c r="M39" s="7">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>37</v>
+      </c>
+      <c r="B40" s="13">
+        <f>MIN(E40,H40,K40)</f>
+        <v>47</v>
+      </c>
+      <c r="C40" s="6">
+        <f>MIN(F40,I40,L40)</f>
+        <v>26</v>
+      </c>
+      <c r="D40" s="7">
+        <f>MAX(G40,J40,M40)</f>
+        <v>86</v>
+      </c>
+      <c r="E40" s="11">
+        <v>50</v>
+      </c>
+      <c r="F40" s="6">
+        <v>26</v>
+      </c>
+      <c r="G40" s="7">
+        <v>79</v>
+      </c>
+      <c r="H40" s="11">
+        <v>47</v>
+      </c>
+      <c r="I40" s="6">
+        <v>26</v>
+      </c>
+      <c r="J40" s="7">
+        <v>86</v>
+      </c>
+      <c r="K40" s="13">
+        <v>47</v>
+      </c>
+      <c r="L40" s="6">
+        <v>26</v>
+      </c>
+      <c r="M40" s="7">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>38</v>
+      </c>
+      <c r="B41" s="13">
+        <f>MIN(E41,H41,K41)</f>
+        <v>41</v>
+      </c>
+      <c r="C41" s="6">
+        <f>MIN(F41,I41,L41)</f>
+        <v>21</v>
+      </c>
+      <c r="D41" s="7">
+        <f>MAX(G41,J41,M41)</f>
+        <v>76</v>
+      </c>
+      <c r="E41" s="11">
+        <v>52</v>
+      </c>
+      <c r="F41" s="6">
+        <v>23</v>
+      </c>
+      <c r="G41" s="7">
+        <v>76</v>
+      </c>
+      <c r="H41" s="11">
+        <v>41</v>
+      </c>
+      <c r="I41" s="6">
+        <v>21</v>
+      </c>
+      <c r="J41" s="7">
+        <v>70</v>
+      </c>
+      <c r="K41" s="13">
+        <v>41</v>
+      </c>
+      <c r="L41" s="6">
+        <v>23</v>
+      </c>
+      <c r="M41" s="7">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>39</v>
+      </c>
+      <c r="B42" s="13">
+        <f>MIN(E42,H42,K42)</f>
+        <v>38</v>
+      </c>
+      <c r="C42" s="6">
+        <f>MIN(F42,I42,L42)</f>
+        <v>26</v>
+      </c>
+      <c r="D42" s="7">
+        <f>MAX(G42,J42,M42)</f>
+        <v>90</v>
+      </c>
+      <c r="E42" s="11">
+        <v>38</v>
+      </c>
+      <c r="F42" s="6">
+        <v>29</v>
+      </c>
+      <c r="G42" s="7">
+        <v>90</v>
+      </c>
+      <c r="H42" s="11">
+        <v>40</v>
+      </c>
+      <c r="I42" s="6">
+        <v>26</v>
+      </c>
+      <c r="J42" s="7">
+        <v>87</v>
+      </c>
+      <c r="K42" s="13">
+        <v>40</v>
+      </c>
+      <c r="L42" s="6">
+        <v>26</v>
+      </c>
+      <c r="M42" s="7">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>40</v>
+      </c>
+      <c r="B43" s="13">
+        <f>MIN(E43,H43,K43)</f>
+        <v>65</v>
+      </c>
+      <c r="C43" s="6">
+        <f>MIN(F43,I43,L43)</f>
+        <v>32</v>
+      </c>
+      <c r="D43" s="7">
+        <f>MAX(G43,J43,M43)</f>
+        <v>105</v>
+      </c>
+      <c r="E43" s="11">
+        <v>72</v>
+      </c>
+      <c r="F43" s="6">
+        <v>34</v>
+      </c>
+      <c r="G43" s="7">
+        <v>100</v>
+      </c>
+      <c r="H43" s="11">
+        <v>65</v>
+      </c>
+      <c r="I43" s="6">
+        <v>32</v>
+      </c>
+      <c r="J43" s="7">
+        <v>104</v>
+      </c>
+      <c r="K43" s="13">
+        <v>65</v>
+      </c>
+      <c r="L43" s="6">
+        <v>36</v>
+      </c>
+      <c r="M43" s="7">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>41</v>
+      </c>
+      <c r="B44" s="13">
+        <f>MIN(E44,H44,K44)</f>
+        <v>53</v>
+      </c>
+      <c r="C44" s="6">
+        <f>MIN(F44,I44,L44)</f>
+        <v>29</v>
+      </c>
+      <c r="D44" s="7">
+        <f>MAX(G44,J44,M44)</f>
+        <v>88</v>
+      </c>
+      <c r="E44" s="11">
+        <v>53</v>
+      </c>
+      <c r="F44" s="6">
+        <v>32</v>
+      </c>
+      <c r="G44" s="7">
+        <v>88</v>
+      </c>
+      <c r="H44" s="11">
+        <v>53</v>
+      </c>
+      <c r="I44" s="6">
+        <v>29</v>
+      </c>
+      <c r="J44" s="7">
+        <v>88</v>
+      </c>
+      <c r="K44" s="13">
+        <v>53</v>
+      </c>
+      <c r="L44" s="6">
+        <v>29</v>
+      </c>
+      <c r="M44" s="7">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>42</v>
+      </c>
+      <c r="B45" s="13">
+        <f>MIN(E45,H45,K45)</f>
+        <v>57</v>
+      </c>
+      <c r="C45" s="6">
+        <f>MIN(F45,I45,L45)</f>
+        <v>32</v>
+      </c>
+      <c r="D45" s="7">
+        <f>MAX(G45,J45,M45)</f>
+        <v>104</v>
+      </c>
+      <c r="E45" s="11">
+        <v>63</v>
+      </c>
+      <c r="F45" s="6">
+        <v>33</v>
+      </c>
+      <c r="G45" s="7">
+        <v>99</v>
+      </c>
+      <c r="H45" s="11">
+        <v>57</v>
+      </c>
+      <c r="I45" s="6">
+        <v>32</v>
+      </c>
+      <c r="J45" s="7">
+        <v>104</v>
+      </c>
+      <c r="K45" s="13">
+        <v>57</v>
+      </c>
+      <c r="L45" s="6">
+        <v>32</v>
+      </c>
+      <c r="M45" s="7">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>43</v>
+      </c>
+      <c r="B46" s="13">
+        <f>MIN(E46,H46,K46)</f>
+        <v>62</v>
+      </c>
+      <c r="C46" s="6">
+        <f>MIN(F46,I46,L46)</f>
+        <v>31</v>
+      </c>
+      <c r="D46" s="7">
+        <f>MAX(G46,J46,M46)</f>
+        <v>107</v>
+      </c>
+      <c r="E46" s="11">
+        <v>62</v>
+      </c>
+      <c r="F46" s="6">
+        <v>34</v>
+      </c>
+      <c r="G46" s="7">
+        <v>107</v>
+      </c>
+      <c r="H46" s="11">
+        <v>62</v>
+      </c>
+      <c r="I46" s="6">
+        <v>31</v>
+      </c>
+      <c r="J46" s="7">
+        <v>105</v>
+      </c>
+      <c r="K46" s="13">
+        <v>62</v>
+      </c>
+      <c r="L46" s="6">
+        <v>31</v>
+      </c>
+      <c r="M46" s="7">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>44</v>
+      </c>
+      <c r="B47" s="13">
+        <f>MIN(E47,H47,K47)</f>
+        <v>56</v>
+      </c>
+      <c r="C47" s="6">
+        <f>MIN(F47,I47,L47)</f>
+        <v>24</v>
+      </c>
+      <c r="D47" s="7">
+        <f>MAX(G47,J47,M47)</f>
+        <v>83</v>
+      </c>
+      <c r="E47" s="11">
+        <v>56</v>
+      </c>
+      <c r="F47" s="6">
+        <v>28</v>
+      </c>
+      <c r="G47" s="7">
+        <v>83</v>
+      </c>
+      <c r="H47" s="11">
+        <v>56</v>
+      </c>
+      <c r="I47" s="6">
+        <v>24</v>
+      </c>
+      <c r="J47" s="7">
+        <v>81</v>
+      </c>
+      <c r="K47" s="13">
+        <v>56</v>
+      </c>
+      <c r="L47" s="6">
+        <v>25</v>
+      </c>
+      <c r="M47" s="7">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>45</v>
+      </c>
+      <c r="B48" s="13">
+        <f>MIN(E48,H48,K48)</f>
+        <v>53</v>
+      </c>
+      <c r="C48" s="6">
+        <f>MIN(F48,I48,L48)</f>
+        <v>31</v>
+      </c>
+      <c r="D48" s="7">
+        <f>MAX(G48,J48,M48)</f>
+        <v>97</v>
+      </c>
+      <c r="E48" s="11">
+        <v>61</v>
+      </c>
+      <c r="F48" s="6">
+        <v>35</v>
+      </c>
+      <c r="G48" s="7">
+        <v>96</v>
+      </c>
+      <c r="H48" s="11">
+        <v>53</v>
+      </c>
+      <c r="I48" s="6">
+        <v>31</v>
+      </c>
+      <c r="J48" s="7">
+        <v>94</v>
+      </c>
+      <c r="K48" s="13">
+        <v>53</v>
+      </c>
+      <c r="L48" s="6">
+        <v>34</v>
+      </c>
+      <c r="M48" s="7">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>46</v>
+      </c>
+      <c r="B49" s="13">
+        <f>MIN(E49,H49,K49)</f>
+        <v>55</v>
+      </c>
+      <c r="C49" s="6">
+        <f>MIN(F49,I49,L49)</f>
+        <v>30</v>
+      </c>
+      <c r="D49" s="7">
+        <f>MAX(G49,J49,M49)</f>
+        <v>101</v>
+      </c>
+      <c r="E49" s="11">
+        <v>55</v>
+      </c>
+      <c r="F49" s="6">
+        <v>34</v>
+      </c>
+      <c r="G49" s="7">
+        <v>98</v>
+      </c>
+      <c r="H49" s="11">
+        <v>56</v>
+      </c>
+      <c r="I49" s="6">
+        <v>30</v>
+      </c>
+      <c r="J49" s="7">
+        <v>99</v>
+      </c>
+      <c r="K49" s="13">
+        <v>56</v>
+      </c>
+      <c r="L49" s="6">
+        <v>34</v>
+      </c>
+      <c r="M49" s="7">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>47</v>
+      </c>
+      <c r="B50" s="13">
+        <f>MIN(E50,H50,K50)</f>
+        <v>59</v>
+      </c>
+      <c r="C50" s="6">
+        <f>MIN(F50,I50,L50)</f>
+        <v>32</v>
+      </c>
+      <c r="D50" s="7">
+        <f>MAX(G50,J50,M50)</f>
+        <v>102</v>
+      </c>
+      <c r="E50" s="11">
+        <v>59</v>
+      </c>
+      <c r="F50" s="6">
+        <v>34</v>
+      </c>
+      <c r="G50" s="7">
+        <v>99</v>
+      </c>
+      <c r="H50" s="11">
+        <v>61</v>
+      </c>
+      <c r="I50" s="6">
+        <v>32</v>
+      </c>
+      <c r="J50" s="7">
+        <v>102</v>
+      </c>
+      <c r="K50" s="13">
+        <v>61</v>
+      </c>
+      <c r="L50" s="6">
+        <v>32</v>
+      </c>
+      <c r="M50" s="7">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>48</v>
+      </c>
+      <c r="B51" s="13">
+        <f>MIN(E51,H51,K51)</f>
+        <v>46</v>
+      </c>
+      <c r="C51" s="6">
+        <f>MIN(F51,I51,L51)</f>
+        <v>27</v>
+      </c>
+      <c r="D51" s="7">
+        <f>MAX(G51,J51,M51)</f>
+        <v>85</v>
+      </c>
+      <c r="E51" s="11">
+        <v>51</v>
+      </c>
+      <c r="F51" s="6">
+        <v>29</v>
+      </c>
+      <c r="G51" s="7">
+        <v>79</v>
+      </c>
+      <c r="H51" s="11">
+        <v>46</v>
+      </c>
+      <c r="I51" s="6">
+        <v>27</v>
+      </c>
+      <c r="J51" s="7">
+        <v>85</v>
+      </c>
+      <c r="K51" s="13">
+        <v>46</v>
+      </c>
+      <c r="L51" s="6">
+        <v>27</v>
+      </c>
+      <c r="M51" s="7">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>49</v>
+      </c>
+      <c r="B52" s="13">
+        <f>MIN(E52,H52,K52)</f>
+        <v>56</v>
+      </c>
+      <c r="C52" s="6">
+        <f>MIN(F52,I52,L52)</f>
+        <v>35</v>
+      </c>
+      <c r="D52" s="7">
+        <f>MAX(G52,J52,M52)</f>
+        <v>106</v>
+      </c>
+      <c r="E52" s="11">
+        <v>67</v>
+      </c>
+      <c r="F52" s="6">
+        <v>37</v>
+      </c>
+      <c r="G52" s="7">
+        <v>101</v>
+      </c>
+      <c r="H52" s="11">
+        <v>56</v>
+      </c>
+      <c r="I52" s="6">
+        <v>35</v>
+      </c>
+      <c r="J52" s="7">
+        <v>106</v>
+      </c>
+      <c r="K52" s="13">
+        <v>56</v>
+      </c>
+      <c r="L52" s="6">
+        <v>35</v>
+      </c>
+      <c r="M52" s="7">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>50</v>
+      </c>
+      <c r="B53" s="13">
+        <f>MIN(E53,H53,K53)</f>
+        <v>60</v>
+      </c>
+      <c r="C53" s="6">
+        <f>MIN(F53,I53,L53)</f>
+        <v>31</v>
+      </c>
+      <c r="D53" s="7">
+        <f>MAX(G53,J53,M53)</f>
+        <v>105</v>
+      </c>
+      <c r="E53" s="11">
+        <v>62</v>
+      </c>
+      <c r="F53" s="6">
+        <v>33</v>
+      </c>
+      <c r="G53" s="7">
+        <v>103</v>
+      </c>
+      <c r="H53" s="11">
+        <v>60</v>
+      </c>
+      <c r="I53" s="6">
+        <v>31</v>
+      </c>
+      <c r="J53" s="7">
+        <v>105</v>
+      </c>
+      <c r="K53" s="13">
+        <v>60</v>
+      </c>
+      <c r="L53" s="6">
+        <v>31</v>
+      </c>
+      <c r="M53" s="7">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>51</v>
+      </c>
+      <c r="B54" s="13">
+        <f>MIN(E54,H54,K54)</f>
+        <v>87</v>
+      </c>
+      <c r="C54" s="6">
+        <f>MIN(F54,I54,L54)</f>
+        <v>40</v>
+      </c>
+      <c r="D54" s="7">
+        <f>MAX(G54,J54,M54)</f>
+        <v>144</v>
+      </c>
+      <c r="E54" s="11">
+        <v>87</v>
+      </c>
+      <c r="F54" s="6">
+        <v>42</v>
+      </c>
+      <c r="G54" s="7">
+        <v>132</v>
+      </c>
+      <c r="H54" s="11">
+        <v>91</v>
+      </c>
+      <c r="I54" s="6">
+        <v>40</v>
+      </c>
+      <c r="J54" s="7">
+        <v>144</v>
+      </c>
+      <c r="K54" s="13">
+        <v>91</v>
+      </c>
+      <c r="L54" s="6">
+        <v>40</v>
+      </c>
+      <c r="M54" s="7">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>52</v>
+      </c>
+      <c r="B55" s="13">
+        <f>MIN(E55,H55,K55)</f>
+        <v>64</v>
+      </c>
+      <c r="C55" s="6">
+        <f>MIN(F55,I55,L55)</f>
+        <v>37</v>
+      </c>
+      <c r="D55" s="7">
+        <f>MAX(G55,J55,M55)</f>
+        <v>132</v>
+      </c>
+      <c r="E55" s="11">
+        <v>64</v>
+      </c>
+      <c r="F55" s="6">
+        <v>38</v>
+      </c>
+      <c r="G55" s="7">
+        <v>129</v>
+      </c>
+      <c r="H55" s="11">
+        <v>64</v>
+      </c>
+      <c r="I55" s="6">
+        <v>37</v>
+      </c>
+      <c r="J55" s="7">
+        <v>132</v>
+      </c>
+      <c r="K55" s="13">
+        <v>64</v>
+      </c>
+      <c r="L55" s="6">
+        <v>37</v>
+      </c>
+      <c r="M55" s="7">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>53</v>
+      </c>
+      <c r="B56" s="13">
+        <f>MIN(E56,H56,K56)</f>
+        <v>54</v>
+      </c>
+      <c r="C56" s="6">
+        <f>MIN(F56,I56,L56)</f>
+        <v>24</v>
+      </c>
+      <c r="D56" s="7">
+        <f>MAX(G56,J56,M56)</f>
+        <v>91</v>
+      </c>
+      <c r="E56" s="11">
+        <v>57</v>
+      </c>
+      <c r="F56" s="6">
+        <v>32</v>
+      </c>
+      <c r="G56" s="7">
+        <v>89</v>
+      </c>
+      <c r="H56" s="11">
+        <v>54</v>
+      </c>
+      <c r="I56" s="6">
+        <v>24</v>
+      </c>
+      <c r="J56" s="7">
+        <v>83</v>
+      </c>
+      <c r="K56" s="13">
+        <v>54</v>
+      </c>
+      <c r="L56" s="6">
+        <v>31</v>
+      </c>
+      <c r="M56" s="7">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>54</v>
+      </c>
+      <c r="B57" s="13">
+        <f>MIN(E57,H57,K57)</f>
+        <v>58</v>
+      </c>
+      <c r="C57" s="6">
+        <f>MIN(F57,I57,L57)</f>
+        <v>30</v>
+      </c>
+      <c r="D57" s="7">
+        <f>MAX(G57,J57,M57)</f>
+        <v>102</v>
+      </c>
+      <c r="E57" s="11">
+        <v>72</v>
+      </c>
+      <c r="F57" s="6">
+        <v>33</v>
+      </c>
+      <c r="G57" s="7">
+        <v>97</v>
+      </c>
+      <c r="H57" s="11">
+        <v>58</v>
+      </c>
+      <c r="I57" s="6">
+        <v>30</v>
+      </c>
+      <c r="J57" s="7">
+        <v>102</v>
+      </c>
+      <c r="K57" s="13">
+        <v>58</v>
+      </c>
+      <c r="L57" s="6">
+        <v>30</v>
+      </c>
+      <c r="M57" s="7">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>55</v>
+      </c>
+      <c r="B58" s="13">
+        <f>MIN(E58,H58,K58)</f>
+        <v>53</v>
+      </c>
+      <c r="C58" s="6">
+        <f>MIN(F58,I58,L58)</f>
+        <v>28</v>
+      </c>
+      <c r="D58" s="7">
+        <f>MAX(G58,J58,M58)</f>
+        <v>86</v>
+      </c>
+      <c r="E58" s="11">
+        <v>69</v>
+      </c>
+      <c r="F58" s="6">
+        <v>30</v>
+      </c>
+      <c r="G58" s="7">
+        <v>83</v>
+      </c>
+      <c r="H58" s="11">
+        <v>53</v>
+      </c>
+      <c r="I58" s="6">
+        <v>28</v>
+      </c>
+      <c r="J58" s="7">
+        <v>83</v>
+      </c>
+      <c r="K58" s="13">
+        <v>53</v>
+      </c>
+      <c r="L58" s="6">
+        <v>29</v>
+      </c>
+      <c r="M58" s="7">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>56</v>
+      </c>
+      <c r="B59" s="13">
+        <f>MIN(E59,H59,K59)</f>
+        <v>59</v>
+      </c>
+      <c r="C59" s="6">
+        <f>MIN(F59,I59,L59)</f>
+        <v>30</v>
+      </c>
+      <c r="D59" s="7">
+        <f>MAX(G59,J59,M59)</f>
+        <v>104</v>
+      </c>
+      <c r="E59" s="11">
+        <v>66</v>
+      </c>
+      <c r="F59" s="6">
+        <v>32</v>
+      </c>
+      <c r="G59" s="7">
+        <v>98</v>
+      </c>
+      <c r="H59" s="11">
+        <v>59</v>
+      </c>
+      <c r="I59" s="6">
+        <v>30</v>
+      </c>
+      <c r="J59" s="7">
+        <v>99</v>
+      </c>
+      <c r="K59" s="13">
+        <v>59</v>
+      </c>
+      <c r="L59" s="6">
+        <v>32</v>
+      </c>
+      <c r="M59" s="7">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>57</v>
+      </c>
+      <c r="B60" s="13">
+        <f>MIN(E60,H60,K60)</f>
+        <v>66</v>
+      </c>
+      <c r="C60" s="6">
+        <f>MIN(F60,I60,L60)</f>
+        <v>29</v>
+      </c>
+      <c r="D60" s="7">
+        <f>MAX(G60,J60,M60)</f>
+        <v>114</v>
+      </c>
+      <c r="E60" s="11">
+        <v>77</v>
+      </c>
+      <c r="F60" s="6">
+        <v>38</v>
+      </c>
+      <c r="G60" s="7">
+        <v>114</v>
+      </c>
+      <c r="H60" s="11">
+        <v>66</v>
+      </c>
+      <c r="I60" s="6">
+        <v>29</v>
+      </c>
+      <c r="J60" s="7">
+        <v>109</v>
+      </c>
+      <c r="K60" s="13">
+        <v>66</v>
+      </c>
+      <c r="L60" s="6">
+        <v>29</v>
+      </c>
+      <c r="M60" s="7">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E61" s="11">
+        <f>AVERAGE(E3:E60)</f>
+        <v>44.655172413793103</v>
+      </c>
+      <c r="F61" s="6">
+        <f t="shared" ref="F61:M61" si="0">AVERAGE(F3:F60)</f>
+        <v>25.275862068965516</v>
+      </c>
+      <c r="G61" s="7">
+        <f t="shared" si="0"/>
+        <v>75.206896551724142</v>
+      </c>
+      <c r="H61" s="11">
+        <f t="shared" si="0"/>
+        <v>42.482758620689658</v>
+      </c>
+      <c r="I61" s="6">
+        <f t="shared" si="0"/>
+        <v>23.517241379310345</v>
+      </c>
+      <c r="J61" s="7">
+        <f t="shared" si="0"/>
+        <v>75.310344827586206</v>
+      </c>
+      <c r="K61" s="13">
+        <f t="shared" si="0"/>
+        <v>42.482758620689658</v>
+      </c>
+      <c r="L61" s="6">
+        <f t="shared" si="0"/>
+        <v>24.275862068965516</v>
+      </c>
+      <c r="M61" s="7">
+        <f t="shared" si="0"/>
+        <v>76.620689655172413</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E1:E1048576 H1:H1048576 K1:K1048576">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>INDIRECT(ADDRESS(ROW(), MOD(COLUMN(), 3))) = INDIRECT(ADDRESS(ROW(), COLUMN()))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:G1048576 J1:J1048576 M1:M1048576">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>INDIRECT(ADDRESS(ROW(), MOD(COLUMN(), 3) + 3)) = INDIRECT(ADDRESS(ROW(), COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Try with and without RotateOptimize
</commit_message>
<xml_diff>
--- a/src/Sandbox/Comparison.xlsx
+++ b/src/Sandbox/Comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joelv\Desktop\PumpjackPipeOptimizer\src\Sandbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF585B37-2BA1-487D-96F0-C263771089E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361BE3D2-10F4-49B0-B567-5FE9F8D6F7AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-210" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{F3EEF332-D963-44B3-89AD-4C5E1973BCE9}"/>
   </bookViews>
@@ -5389,7 +5389,7 @@
   <dimension ref="A1:Q61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5505,7 +5505,7 @@
         <v>5</v>
       </c>
       <c r="I3" s="6">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J3" s="7">
         <v>22</v>
@@ -5514,7 +5514,7 @@
         <v>5</v>
       </c>
       <c r="L3" s="6">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M3" s="7">
         <v>22</v>
@@ -5528,7 +5528,7 @@
       </c>
       <c r="B4" s="13">
         <f>MIN(E4,H4,K4)</f>
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C4" s="6">
         <f>MIN(F4,I4,L4)</f>
@@ -5536,7 +5536,7 @@
       </c>
       <c r="D4" s="7">
         <f>MAX(G4,J4,M4)</f>
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="E4" s="11">
         <v>76</v>
@@ -5548,22 +5548,22 @@
         <v>105</v>
       </c>
       <c r="H4" s="11">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="I4" s="6">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J4" s="7">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="K4" s="13">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="L4" s="6">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="M4" s="7">
-        <v>105</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -5595,10 +5595,10 @@
         <v>40</v>
       </c>
       <c r="I5" s="6">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J5" s="7">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="K5" s="13">
         <v>40</v>
@@ -5620,11 +5620,11 @@
       </c>
       <c r="C6" s="6">
         <f>MIN(F6,I6,L6)</f>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D6" s="7">
         <f>MAX(G6,J6,M6)</f>
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E6" s="11">
         <v>44</v>
@@ -5639,10 +5639,10 @@
         <v>43</v>
       </c>
       <c r="I6" s="6">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J6" s="7">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="K6" s="13">
         <v>43</v>
@@ -5651,7 +5651,7 @@
         <v>22</v>
       </c>
       <c r="M6" s="7">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -5664,11 +5664,11 @@
       </c>
       <c r="C7" s="6">
         <f>MIN(F7,I7,L7)</f>
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D7" s="7">
         <f>MAX(G7,J7,M7)</f>
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E7" s="11">
         <v>41</v>
@@ -5683,19 +5683,19 @@
         <v>44</v>
       </c>
       <c r="I7" s="6">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="J7" s="7">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K7" s="13">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L7" s="6">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="M7" s="7">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -5704,7 +5704,7 @@
       </c>
       <c r="B8" s="13">
         <f>MIN(E8,H8,K8)</f>
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C8" s="6">
         <f>MIN(F8,I8,L8)</f>
@@ -5724,16 +5724,16 @@
         <v>76</v>
       </c>
       <c r="H8" s="11">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I8" s="6">
         <v>24</v>
       </c>
       <c r="J8" s="7">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K8" s="13">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="L8" s="6">
         <v>24</v>
@@ -5748,7 +5748,7 @@
       </c>
       <c r="B9" s="13">
         <f>MIN(E9,H9,K9)</f>
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" s="6">
         <f>MIN(F9,I9,L9)</f>
@@ -5756,7 +5756,7 @@
       </c>
       <c r="D9" s="7">
         <f>MAX(G9,J9,M9)</f>
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E9" s="11">
         <v>50</v>
@@ -5768,22 +5768,22 @@
         <v>82</v>
       </c>
       <c r="H9" s="11">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I9" s="6">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="J9" s="7">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="K9" s="13">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L9" s="6">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="M9" s="7">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Q9" s="17"/>
     </row>
@@ -5813,19 +5813,19 @@
         <v>58</v>
       </c>
       <c r="H10" s="11">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I10" s="6">
         <v>20</v>
       </c>
       <c r="J10" s="7">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K10" s="13">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="L10" s="6">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="M10" s="7">
         <v>62</v>
@@ -5866,13 +5866,13 @@
         <v>73</v>
       </c>
       <c r="K11" s="13">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L11" s="6">
         <v>24</v>
       </c>
       <c r="M11" s="7">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -5881,7 +5881,7 @@
       </c>
       <c r="B12" s="13">
         <f>MIN(E12,H12,K12)</f>
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C12" s="6">
         <f>MIN(F12,I12,L12)</f>
@@ -5889,7 +5889,7 @@
       </c>
       <c r="D12" s="7">
         <f>MAX(G12,J12,M12)</f>
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E12" s="11">
         <v>40</v>
@@ -5901,22 +5901,22 @@
         <v>84</v>
       </c>
       <c r="H12" s="11">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="I12" s="6">
         <v>30</v>
       </c>
       <c r="J12" s="7">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K12" s="13">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="L12" s="6">
         <v>30</v>
       </c>
       <c r="M12" s="7">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -5929,11 +5929,11 @@
       </c>
       <c r="C13" s="6">
         <f>MIN(F13,I13,L13)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D13" s="7">
         <f>MAX(G13,J13,M13)</f>
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E13" s="11">
         <v>45</v>
@@ -5948,19 +5948,19 @@
         <v>43</v>
       </c>
       <c r="I13" s="6">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J13" s="7">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="K13" s="13">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L13" s="6">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M13" s="7">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -5977,7 +5977,7 @@
       </c>
       <c r="D14" s="7">
         <f>MAX(G14,J14,M14)</f>
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E14" s="11">
         <v>35</v>
@@ -5995,7 +5995,7 @@
         <v>17</v>
       </c>
       <c r="J14" s="7">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="K14" s="13">
         <v>29</v>
@@ -6004,7 +6004,7 @@
         <v>17</v>
       </c>
       <c r="M14" s="7">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -6017,11 +6017,11 @@
       </c>
       <c r="C15" s="6">
         <f>MIN(F15,I15,L15)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D15" s="7">
         <f>MAX(G15,J15,M15)</f>
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E15" s="11">
         <v>42</v>
@@ -6036,19 +6036,19 @@
         <v>32</v>
       </c>
       <c r="I15" s="6">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J15" s="7">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K15" s="13">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="L15" s="6">
         <v>23</v>
       </c>
       <c r="M15" s="7">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -6057,15 +6057,15 @@
       </c>
       <c r="B16" s="13">
         <f>MIN(E16,H16,K16)</f>
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C16" s="6">
         <f>MIN(F16,I16,L16)</f>
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D16" s="7">
         <f>MAX(G16,J16,M16)</f>
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E16" s="11">
         <v>39</v>
@@ -6080,19 +6080,19 @@
         <v>40</v>
       </c>
       <c r="I16" s="6">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="J16" s="7">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="K16" s="13">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="L16" s="6">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="M16" s="7">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -6109,7 +6109,7 @@
       </c>
       <c r="D17" s="7">
         <f>MAX(G17,J17,M17)</f>
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E17" s="11">
         <v>35</v>
@@ -6124,19 +6124,19 @@
         <v>35</v>
       </c>
       <c r="I17" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J17" s="7">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="K17" s="13">
         <v>35</v>
       </c>
       <c r="L17" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M17" s="7">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -6145,7 +6145,7 @@
       </c>
       <c r="B18" s="13">
         <f>MIN(E18,H18,K18)</f>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C18" s="6">
         <f>MIN(F18,I18,L18)</f>
@@ -6153,7 +6153,7 @@
       </c>
       <c r="D18" s="7">
         <f>MAX(G18,J18,M18)</f>
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E18" s="11">
         <v>42</v>
@@ -6165,7 +6165,7 @@
         <v>67</v>
       </c>
       <c r="H18" s="11">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I18" s="6">
         <v>24</v>
@@ -6174,13 +6174,13 @@
         <v>66</v>
       </c>
       <c r="K18" s="13">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="L18" s="6">
         <v>24</v>
       </c>
       <c r="M18" s="7">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -6189,7 +6189,7 @@
       </c>
       <c r="B19" s="13">
         <f>MIN(E19,H19,K19)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C19" s="6">
         <f>MIN(F19,I19,L19)</f>
@@ -6209,22 +6209,22 @@
         <v>38</v>
       </c>
       <c r="H19" s="11">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I19" s="6">
         <v>12</v>
       </c>
       <c r="J19" s="7">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="K19" s="13">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L19" s="6">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M19" s="7">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -6237,11 +6237,11 @@
       </c>
       <c r="C20" s="6">
         <f>MIN(F20,I20,L20)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D20" s="7">
         <f>MAX(G20,J20,M20)</f>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E20" s="11">
         <v>17</v>
@@ -6256,19 +6256,19 @@
         <v>17</v>
       </c>
       <c r="I20" s="6">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J20" s="7">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K20" s="13">
         <v>17</v>
       </c>
       <c r="L20" s="6">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M20" s="7">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -6281,7 +6281,7 @@
       </c>
       <c r="C21" s="6">
         <f>MIN(F21,I21,L21)</f>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D21" s="7">
         <f>MAX(G21,J21,M21)</f>
@@ -6300,19 +6300,19 @@
         <v>14</v>
       </c>
       <c r="I21" s="6">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J21" s="7">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="K21" s="13">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="L21" s="6">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M21" s="7">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -6321,7 +6321,7 @@
       </c>
       <c r="B22" s="13">
         <f>MIN(E22,H22,K22)</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22" s="6">
         <f>MIN(F22,I22,L22)</f>
@@ -6329,7 +6329,7 @@
       </c>
       <c r="D22" s="7">
         <f>MAX(G22,J22,M22)</f>
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E22" s="11">
         <v>21</v>
@@ -6341,22 +6341,22 @@
         <v>50</v>
       </c>
       <c r="H22" s="11">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I22" s="6">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J22" s="7">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="K22" s="13">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L22" s="6">
         <v>16</v>
       </c>
       <c r="M22" s="7">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -6391,16 +6391,16 @@
         <v>7</v>
       </c>
       <c r="J23" s="7">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K23" s="13">
         <v>8</v>
       </c>
       <c r="L23" s="6">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M23" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -6429,7 +6429,7 @@
         <v>64</v>
       </c>
       <c r="H24" s="11">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I24" s="6">
         <v>19</v>
@@ -6441,10 +6441,10 @@
         <v>28</v>
       </c>
       <c r="L24" s="6">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M24" s="7">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -6461,7 +6461,7 @@
       </c>
       <c r="D25" s="7">
         <f>MAX(G25,J25,M25)</f>
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E25" s="11">
         <v>32</v>
@@ -6479,7 +6479,7 @@
         <v>23</v>
       </c>
       <c r="J25" s="7">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="K25" s="13">
         <v>31</v>
@@ -6488,7 +6488,7 @@
         <v>23</v>
       </c>
       <c r="M25" s="7">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -6541,15 +6541,15 @@
       </c>
       <c r="B27" s="13">
         <f>MIN(E27,H27,K27)</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C27" s="6">
         <f>MIN(F27,I27,L27)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D27" s="7">
         <f>MAX(G27,J27,M27)</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E27" s="11">
         <v>13</v>
@@ -6561,22 +6561,22 @@
         <v>28</v>
       </c>
       <c r="H27" s="11">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I27" s="6">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J27" s="7">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K27" s="13">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L27" s="6">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M27" s="7">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -6593,7 +6593,7 @@
       </c>
       <c r="D28" s="7">
         <f>MAX(G28,J28,M28)</f>
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="E28" s="11">
         <v>29</v>
@@ -6605,22 +6605,22 @@
         <v>56</v>
       </c>
       <c r="H28" s="11">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I28" s="6">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J28" s="7">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="K28" s="13">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="L28" s="6">
         <v>19</v>
       </c>
       <c r="M28" s="7">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -6637,7 +6637,7 @@
       </c>
       <c r="D29" s="7">
         <f>MAX(G29,J29,M29)</f>
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E29" s="11">
         <v>26</v>
@@ -6649,22 +6649,22 @@
         <v>47</v>
       </c>
       <c r="H29" s="11">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="I29" s="6">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J29" s="7">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="K29" s="13">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="L29" s="6">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="M29" s="7">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -6673,15 +6673,15 @@
       </c>
       <c r="B30" s="13">
         <f>MIN(E30,H30,K30)</f>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C30" s="6">
         <f>MIN(F30,I30,L30)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D30" s="7">
         <f>MAX(G30,J30,M30)</f>
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E30" s="11">
         <v>27</v>
@@ -6693,22 +6693,22 @@
         <v>50</v>
       </c>
       <c r="H30" s="11">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I30" s="6">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J30" s="7">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K30" s="13">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L30" s="6">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M30" s="7">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -6721,11 +6721,11 @@
       </c>
       <c r="C31" s="6">
         <f>MIN(F31,I31,L31)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D31" s="7">
         <f>MAX(G31,J31,M31)</f>
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E31" s="11">
         <v>39</v>
@@ -6740,19 +6740,19 @@
         <v>38</v>
       </c>
       <c r="I31" s="6">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="J31" s="7">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="K31" s="13">
         <v>38</v>
       </c>
       <c r="L31" s="6">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="M31" s="7">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -6765,7 +6765,7 @@
       </c>
       <c r="C32" s="6">
         <f>MIN(F32,I32,L32)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D32" s="7">
         <f>MAX(G32,J32,M32)</f>
@@ -6784,19 +6784,19 @@
         <v>30</v>
       </c>
       <c r="I32" s="6">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J32" s="7">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K32" s="13">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="L32" s="6">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="M32" s="7">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -6805,11 +6805,11 @@
       </c>
       <c r="B33" s="13">
         <f>MIN(E33,H33,K33)</f>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C33" s="6">
         <f>MIN(F33,I33,L33)</f>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D33" s="7">
         <f>MAX(G33,J33,M33)</f>
@@ -6825,19 +6825,19 @@
         <v>68</v>
       </c>
       <c r="H33" s="11">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="I33" s="6">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="J33" s="7">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K33" s="13">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="L33" s="6">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="M33" s="7">
         <v>69</v>
@@ -6853,7 +6853,7 @@
       </c>
       <c r="C34" s="6">
         <f>MIN(F34,I34,L34)</f>
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D34" s="7">
         <f>MAX(G34,J34,M34)</f>
@@ -6872,7 +6872,7 @@
         <v>27</v>
       </c>
       <c r="I34" s="6">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J34" s="7">
         <v>58</v>
@@ -6881,10 +6881,10 @@
         <v>27</v>
       </c>
       <c r="L34" s="6">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M34" s="7">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -6897,11 +6897,11 @@
       </c>
       <c r="C35" s="6">
         <f>MIN(F35,I35,L35)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D35" s="7">
         <f>MAX(G35,J35,M35)</f>
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E35" s="11">
         <v>20</v>
@@ -6916,19 +6916,19 @@
         <v>19</v>
       </c>
       <c r="I35" s="6">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J35" s="7">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K35" s="13">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L35" s="6">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M35" s="7">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
@@ -6937,7 +6937,7 @@
       </c>
       <c r="B36" s="13">
         <f>MIN(E36,H36,K36)</f>
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C36" s="6">
         <f>MIN(F36,I36,L36)</f>
@@ -6957,19 +6957,19 @@
         <v>101</v>
       </c>
       <c r="H36" s="11">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I36" s="6">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J36" s="7">
         <v>108</v>
       </c>
       <c r="K36" s="13">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="L36" s="6">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M36" s="7">
         <v>109</v>
@@ -6985,11 +6985,11 @@
       </c>
       <c r="C37" s="6">
         <f>MIN(F37,I37,L37)</f>
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D37" s="7">
         <f>MAX(G37,J37,M37)</f>
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="E37" s="11">
         <v>75</v>
@@ -7001,22 +7001,22 @@
         <v>118</v>
       </c>
       <c r="H37" s="11">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="I37" s="6">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J37" s="7">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="K37" s="13">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="L37" s="6">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M37" s="7">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -7025,15 +7025,15 @@
       </c>
       <c r="B38" s="13">
         <f>MIN(E38,H38,K38)</f>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C38" s="6">
         <f>MIN(F38,I38,L38)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D38" s="7">
         <f>MAX(G38,J38,M38)</f>
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E38" s="11">
         <v>46</v>
@@ -7045,22 +7045,22 @@
         <v>61</v>
       </c>
       <c r="H38" s="11">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I38" s="6">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J38" s="7">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K38" s="13">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L38" s="6">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M38" s="7">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -7069,15 +7069,15 @@
       </c>
       <c r="B39" s="13">
         <f>MIN(E39,H39,K39)</f>
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C39" s="6">
         <f>MIN(F39,I39,L39)</f>
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D39" s="7">
         <f>MAX(G39,J39,M39)</f>
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="E39" s="11">
         <v>51</v>
@@ -7089,22 +7089,22 @@
         <v>85</v>
       </c>
       <c r="H39" s="11">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="I39" s="6">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J39" s="7">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="K39" s="13">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L39" s="6">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="M39" s="7">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -7113,7 +7113,7 @@
       </c>
       <c r="B40" s="13">
         <f>MIN(E40,H40,K40)</f>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C40" s="6">
         <f>MIN(F40,I40,L40)</f>
@@ -7121,7 +7121,7 @@
       </c>
       <c r="D40" s="7">
         <f>MAX(G40,J40,M40)</f>
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E40" s="11">
         <v>50</v>
@@ -7133,22 +7133,22 @@
         <v>79</v>
       </c>
       <c r="H40" s="11">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I40" s="6">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J40" s="7">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K40" s="13">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L40" s="6">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M40" s="7">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -7161,7 +7161,7 @@
       </c>
       <c r="C41" s="6">
         <f>MIN(F41,I41,L41)</f>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D41" s="7">
         <f>MAX(G41,J41,M41)</f>
@@ -7177,13 +7177,13 @@
         <v>76</v>
       </c>
       <c r="H41" s="11">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="I41" s="6">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="J41" s="7">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="K41" s="13">
         <v>41</v>
@@ -7209,7 +7209,7 @@
       </c>
       <c r="D42" s="7">
         <f>MAX(G42,J42,M42)</f>
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E42" s="11">
         <v>38</v>
@@ -7227,16 +7227,16 @@
         <v>26</v>
       </c>
       <c r="J42" s="7">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="K42" s="13">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L42" s="6">
         <v>26</v>
       </c>
       <c r="M42" s="7">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -7245,15 +7245,15 @@
       </c>
       <c r="B43" s="13">
         <f>MIN(E43,H43,K43)</f>
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C43" s="6">
         <f>MIN(F43,I43,L43)</f>
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D43" s="7">
         <f>MAX(G43,J43,M43)</f>
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E43" s="11">
         <v>72</v>
@@ -7265,22 +7265,22 @@
         <v>100</v>
       </c>
       <c r="H43" s="11">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="I43" s="6">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J43" s="7">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K43" s="13">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="L43" s="6">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M43" s="7">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -7293,11 +7293,11 @@
       </c>
       <c r="C44" s="6">
         <f>MIN(F44,I44,L44)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D44" s="7">
         <f>MAX(G44,J44,M44)</f>
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E44" s="11">
         <v>53</v>
@@ -7312,19 +7312,19 @@
         <v>53</v>
       </c>
       <c r="I44" s="6">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J44" s="7">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K44" s="13">
         <v>53</v>
       </c>
       <c r="L44" s="6">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M44" s="7">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
@@ -7333,15 +7333,15 @@
       </c>
       <c r="B45" s="13">
         <f>MIN(E45,H45,K45)</f>
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C45" s="6">
         <f>MIN(F45,I45,L45)</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D45" s="7">
         <f>MAX(G45,J45,M45)</f>
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="E45" s="11">
         <v>63</v>
@@ -7353,22 +7353,22 @@
         <v>99</v>
       </c>
       <c r="H45" s="11">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I45" s="6">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J45" s="7">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="K45" s="13">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="L45" s="6">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M45" s="7">
-        <v>104</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
@@ -7377,15 +7377,15 @@
       </c>
       <c r="B46" s="13">
         <f>MIN(E46,H46,K46)</f>
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C46" s="6">
         <f>MIN(F46,I46,L46)</f>
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D46" s="7">
         <f>MAX(G46,J46,M46)</f>
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E46" s="11">
         <v>62</v>
@@ -7397,22 +7397,22 @@
         <v>107</v>
       </c>
       <c r="H46" s="11">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I46" s="6">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J46" s="7">
         <v>105</v>
       </c>
       <c r="K46" s="13">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L46" s="6">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="M46" s="7">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
@@ -7421,15 +7421,15 @@
       </c>
       <c r="B47" s="13">
         <f>MIN(E47,H47,K47)</f>
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C47" s="6">
         <f>MIN(F47,I47,L47)</f>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D47" s="7">
         <f>MAX(G47,J47,M47)</f>
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="E47" s="11">
         <v>56</v>
@@ -7441,22 +7441,22 @@
         <v>83</v>
       </c>
       <c r="H47" s="11">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I47" s="6">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J47" s="7">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K47" s="13">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L47" s="6">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M47" s="7">
-        <v>83</v>
+        <v>89</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
@@ -7469,11 +7469,11 @@
       </c>
       <c r="C48" s="6">
         <f>MIN(F48,I48,L48)</f>
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D48" s="7">
         <f>MAX(G48,J48,M48)</f>
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E48" s="11">
         <v>61</v>
@@ -7488,19 +7488,19 @@
         <v>53</v>
       </c>
       <c r="I48" s="6">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J48" s="7">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="K48" s="13">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="L48" s="6">
         <v>34</v>
       </c>
       <c r="M48" s="7">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
@@ -7509,15 +7509,15 @@
       </c>
       <c r="B49" s="13">
         <f>MIN(E49,H49,K49)</f>
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C49" s="6">
         <f>MIN(F49,I49,L49)</f>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D49" s="7">
         <f>MAX(G49,J49,M49)</f>
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="E49" s="11">
         <v>55</v>
@@ -7529,22 +7529,22 @@
         <v>98</v>
       </c>
       <c r="H49" s="11">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="I49" s="6">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J49" s="7">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="K49" s="13">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="L49" s="6">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M49" s="7">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
@@ -7557,11 +7557,11 @@
       </c>
       <c r="C50" s="6">
         <f>MIN(F50,I50,L50)</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D50" s="7">
         <f>MAX(G50,J50,M50)</f>
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E50" s="11">
         <v>59</v>
@@ -7573,22 +7573,22 @@
         <v>99</v>
       </c>
       <c r="H50" s="11">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="I50" s="6">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J50" s="7">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="K50" s="13">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="L50" s="6">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="M50" s="7">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
@@ -7605,7 +7605,7 @@
       </c>
       <c r="D51" s="7">
         <f>MAX(G51,J51,M51)</f>
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E51" s="11">
         <v>51</v>
@@ -7623,7 +7623,7 @@
         <v>27</v>
       </c>
       <c r="J51" s="7">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="K51" s="13">
         <v>46</v>
@@ -7632,7 +7632,7 @@
         <v>27</v>
       </c>
       <c r="M51" s="7">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
@@ -7645,7 +7645,7 @@
       </c>
       <c r="C52" s="6">
         <f>MIN(F52,I52,L52)</f>
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D52" s="7">
         <f>MAX(G52,J52,M52)</f>
@@ -7661,19 +7661,19 @@
         <v>101</v>
       </c>
       <c r="H52" s="11">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I52" s="6">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="J52" s="7">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K52" s="13">
         <v>56</v>
       </c>
       <c r="L52" s="6">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="M52" s="7">
         <v>106</v>
@@ -7685,15 +7685,15 @@
       </c>
       <c r="B53" s="13">
         <f>MIN(E53,H53,K53)</f>
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C53" s="6">
         <f>MIN(F53,I53,L53)</f>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D53" s="7">
         <f>MAX(G53,J53,M53)</f>
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E53" s="11">
         <v>62</v>
@@ -7705,22 +7705,22 @@
         <v>103</v>
       </c>
       <c r="H53" s="11">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="I53" s="6">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J53" s="7">
         <v>105</v>
       </c>
       <c r="K53" s="13">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="L53" s="6">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M53" s="7">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
@@ -7733,11 +7733,11 @@
       </c>
       <c r="C54" s="6">
         <f>MIN(F54,I54,L54)</f>
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D54" s="7">
         <f>MAX(G54,J54,M54)</f>
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E54" s="11">
         <v>87</v>
@@ -7749,22 +7749,22 @@
         <v>132</v>
       </c>
       <c r="H54" s="11">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I54" s="6">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="J54" s="7">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="K54" s="13">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L54" s="6">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="M54" s="7">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
@@ -7777,11 +7777,11 @@
       </c>
       <c r="C55" s="6">
         <f>MIN(F55,I55,L55)</f>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D55" s="7">
         <f>MAX(G55,J55,M55)</f>
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="E55" s="11">
         <v>64</v>
@@ -7796,19 +7796,19 @@
         <v>64</v>
       </c>
       <c r="I55" s="6">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="J55" s="7">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="K55" s="13">
         <v>64</v>
       </c>
       <c r="L55" s="6">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="M55" s="7">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
@@ -7817,15 +7817,15 @@
       </c>
       <c r="B56" s="13">
         <f>MIN(E56,H56,K56)</f>
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C56" s="6">
         <f>MIN(F56,I56,L56)</f>
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D56" s="7">
         <f>MAX(G56,J56,M56)</f>
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E56" s="11">
         <v>57</v>
@@ -7837,22 +7837,22 @@
         <v>89</v>
       </c>
       <c r="H56" s="11">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I56" s="6">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="J56" s="7">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="K56" s="13">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L56" s="6">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M56" s="7">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
@@ -7861,15 +7861,15 @@
       </c>
       <c r="B57" s="13">
         <f>MIN(E57,H57,K57)</f>
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="C57" s="6">
         <f>MIN(F57,I57,L57)</f>
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D57" s="7">
         <f>MAX(G57,J57,M57)</f>
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E57" s="11">
         <v>72</v>
@@ -7881,22 +7881,22 @@
         <v>97</v>
       </c>
       <c r="H57" s="11">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="I57" s="6">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="J57" s="7">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="K57" s="13">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="L57" s="6">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="M57" s="7">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
@@ -7909,7 +7909,7 @@
       </c>
       <c r="C58" s="6">
         <f>MIN(F58,I58,L58)</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D58" s="7">
         <f>MAX(G58,J58,M58)</f>
@@ -7928,10 +7928,10 @@
         <v>53</v>
       </c>
       <c r="I58" s="6">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J58" s="7">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="K58" s="13">
         <v>53</v>
@@ -7953,7 +7953,7 @@
       </c>
       <c r="C59" s="6">
         <f>MIN(F59,I59,L59)</f>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D59" s="7">
         <f>MAX(G59,J59,M59)</f>
@@ -7969,13 +7969,13 @@
         <v>98</v>
       </c>
       <c r="H59" s="11">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I59" s="6">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J59" s="7">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="K59" s="13">
         <v>59</v>
@@ -7993,15 +7993,15 @@
       </c>
       <c r="B60" s="13">
         <f>MIN(E60,H60,K60)</f>
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C60" s="6">
         <f>MIN(F60,I60,L60)</f>
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D60" s="7">
         <f>MAX(G60,J60,M60)</f>
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E60" s="11">
         <v>77</v>
@@ -8013,22 +8013,22 @@
         <v>114</v>
       </c>
       <c r="H60" s="11">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="I60" s="6">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="J60" s="7">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="K60" s="13">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="L60" s="6">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="M60" s="7">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
@@ -8046,27 +8046,27 @@
       </c>
       <c r="H61" s="11">
         <f t="shared" si="0"/>
-        <v>42.482758620689658</v>
+        <v>42.896551724137929</v>
       </c>
       <c r="I61" s="6">
         <f t="shared" si="0"/>
-        <v>23.517241379310345</v>
+        <v>25.120689655172413</v>
       </c>
       <c r="J61" s="7">
         <f t="shared" si="0"/>
-        <v>75.310344827586206</v>
+        <v>77.431034482758619</v>
       </c>
       <c r="K61" s="13">
         <f t="shared" si="0"/>
-        <v>42.482758620689658</v>
+        <v>43.155172413793103</v>
       </c>
       <c r="L61" s="6">
         <f t="shared" si="0"/>
-        <v>24.275862068965516</v>
+        <v>25.396551724137932</v>
       </c>
       <c r="M61" s="7">
         <f t="shared" si="0"/>
-        <v>76.620689655172413</v>
+        <v>78.431034482758619</v>
       </c>
     </row>
   </sheetData>

</xml_diff>